<commit_message>
Completed customer bulk upload
</commit_message>
<xml_diff>
--- a/src/assets/Download/CustomerMasterTemplate.xlsx
+++ b/src/assets/Download/CustomerMasterTemplate.xlsx
@@ -1309,10 +1309,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R290"/>
+  <dimension ref="A1:R286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1470,1137 +1470,1121 @@
       <c r="F7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="6:12">
+    <row r="8" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="6:12">
+    <row r="9" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="6:12">
+    <row r="10" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F10" s="6"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="6:12">
+    <row r="11" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="6:12">
+    <row r="12" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="6:12">
+    <row r="13" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F13" s="6"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="6:12">
+    <row r="14" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F14" s="6"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="6:12">
+    <row r="15" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F15" s="6"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="6:12">
+    <row r="16" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F16" s="6"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" s="1" customFormat="1" spans="6:12">
+    <row r="17" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F17" s="6"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" s="1" customFormat="1" spans="6:12">
+    <row r="18" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F18" s="6"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" s="1" customFormat="1" spans="6:12">
+    <row r="19" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F19" s="6"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" s="1" customFormat="1" spans="6:12">
+    <row r="20" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F20" s="6"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" s="1" customFormat="1" spans="6:12">
+    <row r="21" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F21" s="6"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" s="1" customFormat="1" spans="6:12">
+    <row r="22" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F22" s="6"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" s="1" customFormat="1" spans="6:12">
+    <row r="23" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F23" s="6"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" s="1" customFormat="1" spans="6:12">
+    <row r="24" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F24" s="6"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" s="1" customFormat="1" spans="6:12">
+    <row r="25" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F25" s="6"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" s="1" customFormat="1" spans="6:12">
+    <row r="26" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F26" s="6"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" s="1" customFormat="1" spans="6:12">
+    <row r="27" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F27" s="6"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" s="1" customFormat="1" spans="6:12">
+    <row r="28" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F28" s="6"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" s="1" customFormat="1" spans="6:12">
+    <row r="29" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F29" s="6"/>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" s="1" customFormat="1" spans="6:12">
+    <row r="30" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F30" s="6"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" s="1" customFormat="1" spans="6:12">
+    <row r="31" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F31" s="6"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" s="1" customFormat="1" spans="6:12">
+    <row r="32" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F32" s="6"/>
       <c r="L32" s="6"/>
     </row>
-    <row r="33" s="1" customFormat="1" spans="6:12">
+    <row r="33" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F33" s="6"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" s="1" customFormat="1" spans="6:12">
+    <row r="34" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F34" s="6"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" s="1" customFormat="1" spans="6:12">
+    <row r="35" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F35" s="6"/>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" s="1" customFormat="1" spans="6:12">
+    <row r="36" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F36" s="6"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" s="1" customFormat="1" spans="6:12">
+    <row r="37" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F37" s="6"/>
       <c r="L37" s="6"/>
     </row>
-    <row r="38" s="1" customFormat="1" spans="6:12">
+    <row r="38" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F38" s="6"/>
       <c r="L38" s="6"/>
     </row>
-    <row r="39" s="1" customFormat="1" spans="6:12">
+    <row r="39" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F39" s="6"/>
       <c r="L39" s="6"/>
     </row>
-    <row r="40" s="1" customFormat="1" spans="6:12">
+    <row r="40" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F40" s="6"/>
       <c r="L40" s="6"/>
     </row>
-    <row r="41" s="1" customFormat="1" spans="6:12">
+    <row r="41" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F41" s="6"/>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" s="1" customFormat="1" spans="6:12">
+    <row r="42" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F42" s="6"/>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" s="1" customFormat="1" spans="6:12">
+    <row r="43" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F43" s="6"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" s="1" customFormat="1" spans="6:12">
+    <row r="44" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F44" s="6"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" s="1" customFormat="1" spans="6:12">
+    <row r="45" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F45" s="6"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" s="1" customFormat="1" spans="6:12">
+    <row r="46" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F46" s="6"/>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" s="1" customFormat="1" spans="6:12">
+    <row r="47" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F47" s="6"/>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" s="1" customFormat="1" spans="6:12">
+    <row r="48" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F48" s="6"/>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" s="1" customFormat="1" spans="6:12">
+    <row r="49" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F49" s="6"/>
       <c r="L49" s="6"/>
     </row>
-    <row r="50" s="1" customFormat="1" spans="6:12">
+    <row r="50" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F50" s="6"/>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" s="1" customFormat="1" spans="6:12">
+    <row r="51" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F51" s="6"/>
       <c r="L51" s="6"/>
     </row>
-    <row r="52" s="1" customFormat="1" spans="6:12">
+    <row r="52" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F52" s="6"/>
       <c r="L52" s="6"/>
     </row>
-    <row r="53" s="1" customFormat="1" spans="6:12">
+    <row r="53" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F53" s="6"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" s="1" customFormat="1" spans="6:12">
+    <row r="54" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F54" s="6"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" s="1" customFormat="1" spans="6:12">
+    <row r="55" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F55" s="6"/>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" s="1" customFormat="1" spans="6:12">
+    <row r="56" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F56" s="6"/>
       <c r="L56" s="6"/>
     </row>
-    <row r="57" s="1" customFormat="1" spans="6:12">
+    <row r="57" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F57" s="6"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" s="1" customFormat="1" spans="6:12">
+    <row r="58" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F58" s="6"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" s="1" customFormat="1" spans="6:12">
+    <row r="59" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F59" s="6"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" s="1" customFormat="1" spans="6:12">
+    <row r="60" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F60" s="6"/>
       <c r="L60" s="6"/>
     </row>
-    <row r="61" s="1" customFormat="1" spans="6:12">
+    <row r="61" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F61" s="6"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" s="1" customFormat="1" spans="6:12">
+    <row r="62" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F62" s="6"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" s="1" customFormat="1" spans="6:12">
+    <row r="63" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F63" s="6"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" s="1" customFormat="1" spans="6:12">
+    <row r="64" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F64" s="6"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" s="1" customFormat="1" spans="6:12">
+    <row r="65" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F65" s="6"/>
       <c r="L65" s="6"/>
     </row>
-    <row r="66" s="1" customFormat="1" spans="6:12">
+    <row r="66" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F66" s="6"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" s="1" customFormat="1" spans="6:12">
+    <row r="67" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F67" s="6"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" s="1" customFormat="1" spans="6:12">
+    <row r="68" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F68" s="6"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" s="1" customFormat="1" spans="6:12">
+    <row r="69" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F69" s="6"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" s="1" customFormat="1" spans="6:12">
+    <row r="70" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F70" s="6"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" s="1" customFormat="1" spans="6:12">
+    <row r="71" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F71" s="6"/>
       <c r="L71" s="6"/>
     </row>
-    <row r="72" s="1" customFormat="1" spans="6:12">
+    <row r="72" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F72" s="6"/>
       <c r="L72" s="6"/>
     </row>
-    <row r="73" s="1" customFormat="1" spans="6:12">
+    <row r="73" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F73" s="6"/>
       <c r="L73" s="6"/>
     </row>
-    <row r="74" s="1" customFormat="1" spans="6:12">
+    <row r="74" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F74" s="6"/>
       <c r="L74" s="6"/>
     </row>
-    <row r="75" s="1" customFormat="1" spans="6:12">
+    <row r="75" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F75" s="6"/>
       <c r="L75" s="6"/>
     </row>
-    <row r="76" s="1" customFormat="1" spans="6:12">
+    <row r="76" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F76" s="6"/>
       <c r="L76" s="6"/>
     </row>
-    <row r="77" s="1" customFormat="1" spans="6:12">
+    <row r="77" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F77" s="6"/>
       <c r="L77" s="6"/>
     </row>
-    <row r="78" s="1" customFormat="1" spans="6:12">
+    <row r="78" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F78" s="6"/>
       <c r="L78" s="6"/>
     </row>
-    <row r="79" s="1" customFormat="1" spans="6:12">
+    <row r="79" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F79" s="6"/>
       <c r="L79" s="6"/>
     </row>
-    <row r="80" s="1" customFormat="1" spans="6:12">
+    <row r="80" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F80" s="6"/>
       <c r="L80" s="6"/>
     </row>
-    <row r="81" s="1" customFormat="1" spans="6:12">
+    <row r="81" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F81" s="6"/>
       <c r="L81" s="6"/>
     </row>
-    <row r="82" s="1" customFormat="1" spans="6:12">
+    <row r="82" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F82" s="6"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" s="1" customFormat="1" spans="6:12">
+    <row r="83" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F83" s="6"/>
       <c r="L83" s="6"/>
     </row>
-    <row r="84" s="1" customFormat="1" spans="6:12">
+    <row r="84" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F84" s="6"/>
       <c r="L84" s="6"/>
     </row>
-    <row r="85" s="1" customFormat="1" spans="6:12">
+    <row r="85" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F85" s="6"/>
       <c r="L85" s="6"/>
     </row>
-    <row r="86" s="1" customFormat="1" spans="6:12">
+    <row r="86" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F86" s="6"/>
       <c r="L86" s="6"/>
     </row>
-    <row r="87" s="1" customFormat="1" spans="6:12">
+    <row r="87" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F87" s="6"/>
       <c r="L87" s="6"/>
     </row>
-    <row r="88" s="1" customFormat="1" spans="6:12">
+    <row r="88" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F88" s="6"/>
       <c r="L88" s="6"/>
     </row>
-    <row r="89" s="1" customFormat="1" spans="6:12">
+    <row r="89" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F89" s="6"/>
       <c r="L89" s="6"/>
     </row>
-    <row r="90" s="1" customFormat="1" spans="6:12">
+    <row r="90" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F90" s="6"/>
       <c r="L90" s="6"/>
     </row>
-    <row r="91" s="1" customFormat="1" spans="6:12">
+    <row r="91" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F91" s="6"/>
       <c r="L91" s="6"/>
     </row>
-    <row r="92" s="1" customFormat="1" spans="6:12">
+    <row r="92" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F92" s="6"/>
       <c r="L92" s="6"/>
     </row>
-    <row r="93" s="1" customFormat="1" spans="6:12">
+    <row r="93" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F93" s="6"/>
       <c r="L93" s="6"/>
     </row>
-    <row r="94" s="1" customFormat="1" spans="6:12">
+    <row r="94" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F94" s="6"/>
       <c r="L94" s="6"/>
     </row>
-    <row r="95" s="1" customFormat="1" spans="6:12">
+    <row r="95" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F95" s="6"/>
       <c r="L95" s="6"/>
     </row>
-    <row r="96" s="1" customFormat="1" spans="6:12">
+    <row r="96" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F96" s="6"/>
       <c r="L96" s="6"/>
     </row>
-    <row r="97" s="1" customFormat="1" spans="6:12">
+    <row r="97" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F97" s="6"/>
       <c r="L97" s="6"/>
     </row>
-    <row r="98" s="1" customFormat="1" spans="6:12">
+    <row r="98" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F98" s="6"/>
       <c r="L98" s="6"/>
     </row>
-    <row r="99" s="1" customFormat="1" spans="6:12">
+    <row r="99" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F99" s="6"/>
       <c r="L99" s="6"/>
     </row>
-    <row r="100" s="1" customFormat="1" spans="6:12">
+    <row r="100" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F100" s="6"/>
       <c r="L100" s="6"/>
     </row>
-    <row r="101" s="1" customFormat="1" spans="6:12">
+    <row r="101" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F101" s="6"/>
       <c r="L101" s="6"/>
     </row>
-    <row r="102" s="1" customFormat="1" spans="6:12">
+    <row r="102" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F102" s="6"/>
       <c r="L102" s="6"/>
     </row>
-    <row r="103" s="1" customFormat="1" spans="6:12">
+    <row r="103" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F103" s="6"/>
       <c r="L103" s="6"/>
     </row>
-    <row r="104" s="1" customFormat="1" spans="6:12">
+    <row r="104" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F104" s="6"/>
       <c r="L104" s="6"/>
     </row>
-    <row r="105" s="1" customFormat="1" spans="6:12">
+    <row r="105" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F105" s="6"/>
       <c r="L105" s="6"/>
     </row>
-    <row r="106" s="1" customFormat="1" spans="6:12">
+    <row r="106" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F106" s="6"/>
       <c r="L106" s="6"/>
     </row>
-    <row r="107" s="1" customFormat="1" spans="6:12">
+    <row r="107" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F107" s="6"/>
       <c r="L107" s="6"/>
     </row>
-    <row r="108" s="1" customFormat="1" spans="6:12">
+    <row r="108" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F108" s="6"/>
       <c r="L108" s="6"/>
     </row>
-    <row r="109" s="1" customFormat="1" spans="6:12">
+    <row r="109" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F109" s="6"/>
       <c r="L109" s="6"/>
     </row>
-    <row r="110" s="1" customFormat="1" spans="6:12">
+    <row r="110" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F110" s="6"/>
       <c r="L110" s="6"/>
     </row>
-    <row r="111" s="1" customFormat="1" spans="6:12">
+    <row r="111" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F111" s="6"/>
       <c r="L111" s="6"/>
     </row>
-    <row r="112" s="1" customFormat="1" spans="6:12">
+    <row r="112" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F112" s="6"/>
       <c r="L112" s="6"/>
     </row>
-    <row r="113" s="1" customFormat="1" spans="6:12">
+    <row r="113" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F113" s="6"/>
       <c r="L113" s="6"/>
     </row>
-    <row r="114" s="1" customFormat="1" spans="6:12">
+    <row r="114" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F114" s="6"/>
       <c r="L114" s="6"/>
     </row>
-    <row r="115" s="1" customFormat="1" spans="6:12">
+    <row r="115" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F115" s="6"/>
       <c r="L115" s="6"/>
     </row>
-    <row r="116" s="1" customFormat="1" spans="6:12">
+    <row r="116" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F116" s="6"/>
       <c r="L116" s="6"/>
     </row>
-    <row r="117" s="1" customFormat="1" spans="6:12">
+    <row r="117" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F117" s="6"/>
       <c r="L117" s="6"/>
     </row>
-    <row r="118" s="1" customFormat="1" spans="6:12">
+    <row r="118" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F118" s="6"/>
       <c r="L118" s="6"/>
     </row>
-    <row r="119" s="1" customFormat="1" spans="6:12">
+    <row r="119" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F119" s="6"/>
       <c r="L119" s="6"/>
     </row>
-    <row r="120" s="1" customFormat="1" spans="6:12">
+    <row r="120" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F120" s="6"/>
       <c r="L120" s="6"/>
     </row>
-    <row r="121" s="1" customFormat="1" spans="6:12">
+    <row r="121" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F121" s="6"/>
       <c r="L121" s="6"/>
     </row>
-    <row r="122" s="1" customFormat="1" spans="6:12">
+    <row r="122" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F122" s="6"/>
       <c r="L122" s="6"/>
     </row>
-    <row r="123" s="1" customFormat="1" spans="6:12">
+    <row r="123" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F123" s="6"/>
       <c r="L123" s="6"/>
     </row>
-    <row r="124" s="1" customFormat="1" spans="6:12">
+    <row r="124" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F124" s="6"/>
       <c r="L124" s="6"/>
     </row>
-    <row r="125" s="1" customFormat="1" spans="6:12">
+    <row r="125" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F125" s="6"/>
       <c r="L125" s="6"/>
     </row>
-    <row r="126" s="1" customFormat="1" spans="6:12">
+    <row r="126" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F126" s="6"/>
       <c r="L126" s="6"/>
     </row>
-    <row r="127" s="1" customFormat="1" spans="6:12">
+    <row r="127" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F127" s="6"/>
       <c r="L127" s="6"/>
     </row>
-    <row r="128" s="1" customFormat="1" spans="6:12">
+    <row r="128" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F128" s="6"/>
       <c r="L128" s="6"/>
     </row>
-    <row r="129" s="1" customFormat="1" spans="6:12">
+    <row r="129" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F129" s="6"/>
       <c r="L129" s="6"/>
     </row>
-    <row r="130" s="1" customFormat="1" spans="6:12">
+    <row r="130" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F130" s="6"/>
       <c r="L130" s="6"/>
     </row>
-    <row r="131" s="1" customFormat="1" spans="6:12">
+    <row r="131" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F131" s="6"/>
       <c r="L131" s="6"/>
     </row>
-    <row r="132" s="1" customFormat="1" spans="6:12">
+    <row r="132" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F132" s="6"/>
       <c r="L132" s="6"/>
     </row>
-    <row r="133" s="1" customFormat="1" spans="6:12">
+    <row r="133" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F133" s="6"/>
       <c r="L133" s="6"/>
     </row>
-    <row r="134" s="1" customFormat="1" spans="6:12">
+    <row r="134" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F134" s="6"/>
       <c r="L134" s="6"/>
     </row>
-    <row r="135" s="1" customFormat="1" spans="6:12">
+    <row r="135" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F135" s="6"/>
       <c r="L135" s="6"/>
     </row>
-    <row r="136" s="1" customFormat="1" spans="6:12">
+    <row r="136" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F136" s="6"/>
       <c r="L136" s="6"/>
     </row>
-    <row r="137" s="1" customFormat="1" spans="6:12">
+    <row r="137" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F137" s="6"/>
       <c r="L137" s="6"/>
     </row>
-    <row r="138" s="1" customFormat="1" spans="6:12">
+    <row r="138" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F138" s="6"/>
       <c r="L138" s="6"/>
     </row>
-    <row r="139" s="1" customFormat="1" spans="6:12">
+    <row r="139" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F139" s="6"/>
       <c r="L139" s="6"/>
     </row>
-    <row r="140" s="1" customFormat="1" spans="6:12">
+    <row r="140" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F140" s="6"/>
       <c r="L140" s="6"/>
     </row>
-    <row r="141" s="1" customFormat="1" spans="6:12">
+    <row r="141" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F141" s="6"/>
       <c r="L141" s="6"/>
     </row>
-    <row r="142" s="1" customFormat="1" spans="6:12">
+    <row r="142" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F142" s="6"/>
       <c r="L142" s="6"/>
     </row>
-    <row r="143" s="1" customFormat="1" spans="6:12">
+    <row r="143" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F143" s="6"/>
       <c r="L143" s="6"/>
     </row>
-    <row r="144" s="1" customFormat="1" spans="6:12">
+    <row r="144" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F144" s="6"/>
       <c r="L144" s="6"/>
     </row>
-    <row r="145" s="1" customFormat="1" spans="6:12">
+    <row r="145" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F145" s="6"/>
       <c r="L145" s="6"/>
     </row>
-    <row r="146" s="1" customFormat="1" spans="6:12">
+    <row r="146" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F146" s="6"/>
       <c r="L146" s="6"/>
     </row>
-    <row r="147" s="1" customFormat="1" spans="6:12">
+    <row r="147" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F147" s="6"/>
       <c r="L147" s="6"/>
     </row>
-    <row r="148" s="1" customFormat="1" spans="6:12">
+    <row r="148" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F148" s="6"/>
       <c r="L148" s="6"/>
     </row>
-    <row r="149" s="1" customFormat="1" spans="6:12">
+    <row r="149" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F149" s="6"/>
       <c r="L149" s="6"/>
     </row>
-    <row r="150" s="1" customFormat="1" spans="6:12">
+    <row r="150" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F150" s="6"/>
       <c r="L150" s="6"/>
     </row>
-    <row r="151" s="1" customFormat="1" spans="6:12">
+    <row r="151" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F151" s="6"/>
       <c r="L151" s="6"/>
     </row>
-    <row r="152" s="1" customFormat="1" spans="6:12">
+    <row r="152" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F152" s="6"/>
       <c r="L152" s="6"/>
     </row>
-    <row r="153" s="1" customFormat="1" spans="6:12">
+    <row r="153" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F153" s="6"/>
       <c r="L153" s="6"/>
     </row>
-    <row r="154" s="1" customFormat="1" spans="6:12">
+    <row r="154" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F154" s="6"/>
       <c r="L154" s="6"/>
     </row>
-    <row r="155" s="1" customFormat="1" spans="6:12">
+    <row r="155" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F155" s="6"/>
       <c r="L155" s="6"/>
     </row>
-    <row r="156" s="1" customFormat="1" spans="6:12">
+    <row r="156" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F156" s="6"/>
       <c r="L156" s="6"/>
     </row>
-    <row r="157" s="1" customFormat="1" spans="6:12">
+    <row r="157" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F157" s="6"/>
       <c r="L157" s="6"/>
     </row>
-    <row r="158" s="1" customFormat="1" spans="6:12">
+    <row r="158" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F158" s="6"/>
       <c r="L158" s="6"/>
     </row>
-    <row r="159" s="1" customFormat="1" spans="6:12">
+    <row r="159" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F159" s="6"/>
       <c r="L159" s="6"/>
     </row>
-    <row r="160" s="1" customFormat="1" spans="6:12">
+    <row r="160" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F160" s="6"/>
       <c r="L160" s="6"/>
     </row>
-    <row r="161" s="1" customFormat="1" spans="6:12">
+    <row r="161" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F161" s="6"/>
       <c r="L161" s="6"/>
     </row>
-    <row r="162" s="1" customFormat="1" spans="6:12">
+    <row r="162" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F162" s="6"/>
       <c r="L162" s="6"/>
     </row>
-    <row r="163" s="1" customFormat="1" spans="6:12">
+    <row r="163" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F163" s="6"/>
       <c r="L163" s="6"/>
     </row>
-    <row r="164" s="1" customFormat="1" spans="6:12">
+    <row r="164" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F164" s="6"/>
       <c r="L164" s="6"/>
     </row>
-    <row r="165" s="1" customFormat="1" spans="6:12">
+    <row r="165" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F165" s="6"/>
       <c r="L165" s="6"/>
     </row>
-    <row r="166" s="1" customFormat="1" spans="6:12">
+    <row r="166" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F166" s="6"/>
       <c r="L166" s="6"/>
     </row>
-    <row r="167" s="1" customFormat="1" spans="6:12">
+    <row r="167" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F167" s="6"/>
       <c r="L167" s="6"/>
     </row>
-    <row r="168" s="1" customFormat="1" spans="6:12">
+    <row r="168" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F168" s="6"/>
       <c r="L168" s="6"/>
     </row>
-    <row r="169" s="1" customFormat="1" spans="6:12">
+    <row r="169" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F169" s="6"/>
       <c r="L169" s="6"/>
     </row>
-    <row r="170" s="1" customFormat="1" spans="6:12">
+    <row r="170" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F170" s="6"/>
       <c r="L170" s="6"/>
     </row>
-    <row r="171" s="1" customFormat="1" spans="6:12">
+    <row r="171" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F171" s="6"/>
       <c r="L171" s="6"/>
     </row>
-    <row r="172" s="1" customFormat="1" spans="6:12">
+    <row r="172" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F172" s="6"/>
       <c r="L172" s="6"/>
     </row>
-    <row r="173" s="1" customFormat="1" spans="6:12">
+    <row r="173" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F173" s="6"/>
       <c r="L173" s="6"/>
     </row>
-    <row r="174" s="1" customFormat="1" spans="6:12">
+    <row r="174" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F174" s="6"/>
       <c r="L174" s="6"/>
     </row>
-    <row r="175" s="1" customFormat="1" spans="6:12">
+    <row r="175" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F175" s="6"/>
       <c r="L175" s="6"/>
     </row>
-    <row r="176" s="1" customFormat="1" spans="6:12">
+    <row r="176" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F176" s="6"/>
       <c r="L176" s="6"/>
     </row>
-    <row r="177" s="1" customFormat="1" spans="6:12">
+    <row r="177" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F177" s="6"/>
       <c r="L177" s="6"/>
     </row>
-    <row r="178" s="1" customFormat="1" spans="6:12">
+    <row r="178" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F178" s="6"/>
       <c r="L178" s="6"/>
     </row>
-    <row r="179" s="1" customFormat="1" spans="6:12">
+    <row r="179" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F179" s="6"/>
       <c r="L179" s="6"/>
     </row>
-    <row r="180" s="1" customFormat="1" spans="6:12">
+    <row r="180" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F180" s="6"/>
       <c r="L180" s="6"/>
     </row>
-    <row r="181" s="1" customFormat="1" spans="6:12">
+    <row r="181" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F181" s="6"/>
       <c r="L181" s="6"/>
     </row>
-    <row r="182" s="1" customFormat="1" spans="6:12">
+    <row r="182" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F182" s="6"/>
       <c r="L182" s="6"/>
     </row>
-    <row r="183" s="1" customFormat="1" spans="6:12">
+    <row r="183" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F183" s="6"/>
       <c r="L183" s="6"/>
     </row>
-    <row r="184" s="1" customFormat="1" spans="6:12">
+    <row r="184" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F184" s="6"/>
       <c r="L184" s="6"/>
     </row>
-    <row r="185" s="1" customFormat="1" spans="6:12">
+    <row r="185" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F185" s="6"/>
       <c r="L185" s="6"/>
     </row>
-    <row r="186" s="1" customFormat="1" spans="6:12">
+    <row r="186" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F186" s="6"/>
       <c r="L186" s="6"/>
     </row>
-    <row r="187" s="1" customFormat="1" spans="6:12">
+    <row r="187" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F187" s="6"/>
       <c r="L187" s="6"/>
     </row>
-    <row r="188" s="1" customFormat="1" spans="6:12">
+    <row r="188" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F188" s="6"/>
       <c r="L188" s="6"/>
     </row>
-    <row r="189" s="1" customFormat="1" spans="6:12">
+    <row r="189" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F189" s="6"/>
       <c r="L189" s="6"/>
     </row>
-    <row r="190" s="1" customFormat="1" spans="6:12">
+    <row r="190" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F190" s="6"/>
       <c r="L190" s="6"/>
     </row>
-    <row r="191" s="1" customFormat="1" spans="6:12">
+    <row r="191" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F191" s="6"/>
       <c r="L191" s="6"/>
     </row>
-    <row r="192" s="1" customFormat="1" spans="6:12">
+    <row r="192" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F192" s="6"/>
       <c r="L192" s="6"/>
     </row>
-    <row r="193" s="1" customFormat="1" spans="6:12">
+    <row r="193" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F193" s="6"/>
       <c r="L193" s="6"/>
     </row>
-    <row r="194" s="1" customFormat="1" spans="6:12">
+    <row r="194" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F194" s="6"/>
       <c r="L194" s="6"/>
     </row>
-    <row r="195" s="1" customFormat="1" spans="6:12">
+    <row r="195" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F195" s="6"/>
       <c r="L195" s="6"/>
     </row>
-    <row r="196" s="1" customFormat="1" spans="6:12">
+    <row r="196" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F196" s="6"/>
       <c r="L196" s="6"/>
     </row>
-    <row r="197" s="1" customFormat="1" spans="6:12">
+    <row r="197" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F197" s="6"/>
       <c r="L197" s="6"/>
     </row>
-    <row r="198" s="1" customFormat="1" spans="6:12">
+    <row r="198" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F198" s="6"/>
       <c r="L198" s="6"/>
     </row>
-    <row r="199" s="1" customFormat="1" spans="6:12">
+    <row r="199" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F199" s="6"/>
       <c r="L199" s="6"/>
     </row>
-    <row r="200" s="1" customFormat="1" spans="6:12">
+    <row r="200" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F200" s="6"/>
       <c r="L200" s="6"/>
     </row>
-    <row r="201" s="1" customFormat="1" spans="6:12">
+    <row r="201" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F201" s="6"/>
       <c r="L201" s="6"/>
     </row>
-    <row r="202" s="1" customFormat="1" spans="6:12">
+    <row r="202" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F202" s="6"/>
       <c r="L202" s="6"/>
     </row>
-    <row r="203" s="1" customFormat="1" spans="6:12">
+    <row r="203" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F203" s="6"/>
       <c r="L203" s="6"/>
     </row>
-    <row r="204" s="1" customFormat="1" spans="6:12">
+    <row r="204" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F204" s="6"/>
       <c r="L204" s="6"/>
     </row>
-    <row r="205" s="1" customFormat="1" spans="6:12">
+    <row r="205" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F205" s="6"/>
       <c r="L205" s="6"/>
     </row>
-    <row r="206" s="1" customFormat="1" spans="6:12">
+    <row r="206" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F206" s="6"/>
       <c r="L206" s="6"/>
     </row>
-    <row r="207" s="1" customFormat="1" spans="6:12">
+    <row r="207" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F207" s="6"/>
       <c r="L207" s="6"/>
     </row>
-    <row r="208" s="1" customFormat="1" spans="6:12">
+    <row r="208" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F208" s="6"/>
       <c r="L208" s="6"/>
     </row>
-    <row r="209" s="1" customFormat="1" spans="6:12">
+    <row r="209" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F209" s="6"/>
       <c r="L209" s="6"/>
     </row>
-    <row r="210" s="1" customFormat="1" spans="6:12">
+    <row r="210" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F210" s="6"/>
       <c r="L210" s="6"/>
     </row>
-    <row r="211" s="1" customFormat="1" spans="6:12">
+    <row r="211" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F211" s="6"/>
       <c r="L211" s="6"/>
     </row>
-    <row r="212" s="1" customFormat="1" spans="6:12">
+    <row r="212" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F212" s="6"/>
       <c r="L212" s="6"/>
     </row>
-    <row r="213" s="1" customFormat="1" spans="6:12">
+    <row r="213" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F213" s="6"/>
       <c r="L213" s="6"/>
     </row>
-    <row r="214" s="1" customFormat="1" spans="6:12">
+    <row r="214" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F214" s="6"/>
       <c r="L214" s="6"/>
     </row>
-    <row r="215" s="1" customFormat="1" spans="6:12">
+    <row r="215" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F215" s="6"/>
       <c r="L215" s="6"/>
     </row>
-    <row r="216" s="1" customFormat="1" spans="6:12">
+    <row r="216" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F216" s="6"/>
       <c r="L216" s="6"/>
     </row>
-    <row r="217" s="1" customFormat="1" spans="6:12">
+    <row r="217" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F217" s="6"/>
       <c r="L217" s="6"/>
     </row>
-    <row r="218" s="1" customFormat="1" spans="6:12">
+    <row r="218" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F218" s="6"/>
       <c r="L218" s="6"/>
     </row>
-    <row r="219" s="1" customFormat="1" spans="6:12">
+    <row r="219" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F219" s="6"/>
       <c r="L219" s="6"/>
     </row>
-    <row r="220" s="1" customFormat="1" spans="6:12">
+    <row r="220" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F220" s="6"/>
       <c r="L220" s="6"/>
     </row>
-    <row r="221" s="1" customFormat="1" spans="6:12">
+    <row r="221" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F221" s="6"/>
       <c r="L221" s="6"/>
     </row>
-    <row r="222" s="1" customFormat="1" spans="6:12">
+    <row r="222" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F222" s="6"/>
       <c r="L222" s="6"/>
     </row>
-    <row r="223" s="1" customFormat="1" spans="6:12">
+    <row r="223" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F223" s="6"/>
       <c r="L223" s="6"/>
     </row>
-    <row r="224" s="1" customFormat="1" spans="6:12">
+    <row r="224" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F224" s="6"/>
       <c r="L224" s="6"/>
     </row>
-    <row r="225" s="1" customFormat="1" spans="6:12">
+    <row r="225" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F225" s="6"/>
       <c r="L225" s="6"/>
     </row>
-    <row r="226" s="1" customFormat="1" spans="6:12">
+    <row r="226" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F226" s="6"/>
       <c r="L226" s="6"/>
     </row>
-    <row r="227" s="1" customFormat="1" spans="6:12">
+    <row r="227" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F227" s="6"/>
       <c r="L227" s="6"/>
     </row>
-    <row r="228" s="1" customFormat="1" spans="6:12">
+    <row r="228" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F228" s="6"/>
       <c r="L228" s="6"/>
     </row>
-    <row r="229" s="1" customFormat="1" spans="6:12">
+    <row r="229" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F229" s="6"/>
       <c r="L229" s="6"/>
     </row>
-    <row r="230" s="1" customFormat="1" spans="6:12">
+    <row r="230" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F230" s="6"/>
       <c r="L230" s="6"/>
     </row>
-    <row r="231" s="1" customFormat="1" spans="6:12">
+    <row r="231" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F231" s="6"/>
       <c r="L231" s="6"/>
     </row>
-    <row r="232" s="1" customFormat="1" spans="6:12">
+    <row r="232" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F232" s="6"/>
       <c r="L232" s="6"/>
     </row>
-    <row r="233" s="1" customFormat="1" spans="6:12">
+    <row r="233" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F233" s="6"/>
       <c r="L233" s="6"/>
     </row>
-    <row r="234" s="1" customFormat="1" spans="6:12">
+    <row r="234" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F234" s="6"/>
       <c r="L234" s="6"/>
     </row>
-    <row r="235" s="1" customFormat="1" spans="6:12">
+    <row r="235" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F235" s="6"/>
       <c r="L235" s="6"/>
     </row>
-    <row r="236" s="1" customFormat="1" spans="6:12">
+    <row r="236" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F236" s="6"/>
       <c r="L236" s="6"/>
     </row>
-    <row r="237" s="1" customFormat="1" spans="6:12">
+    <row r="237" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F237" s="6"/>
       <c r="L237" s="6"/>
     </row>
-    <row r="238" s="1" customFormat="1" spans="6:12">
+    <row r="238" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F238" s="6"/>
       <c r="L238" s="6"/>
     </row>
-    <row r="239" s="1" customFormat="1" spans="6:12">
+    <row r="239" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F239" s="6"/>
       <c r="L239" s="6"/>
     </row>
-    <row r="240" s="1" customFormat="1" spans="6:12">
+    <row r="240" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F240" s="6"/>
       <c r="L240" s="6"/>
     </row>
-    <row r="241" s="1" customFormat="1" spans="6:12">
+    <row r="241" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F241" s="6"/>
       <c r="L241" s="6"/>
     </row>
-    <row r="242" s="1" customFormat="1" spans="6:12">
+    <row r="242" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F242" s="6"/>
       <c r="L242" s="6"/>
     </row>
-    <row r="243" s="1" customFormat="1" spans="6:12">
+    <row r="243" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F243" s="6"/>
       <c r="L243" s="6"/>
     </row>
-    <row r="244" s="1" customFormat="1" spans="6:12">
+    <row r="244" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F244" s="6"/>
       <c r="L244" s="6"/>
     </row>
-    <row r="245" s="1" customFormat="1" spans="6:12">
+    <row r="245" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F245" s="6"/>
       <c r="L245" s="6"/>
     </row>
-    <row r="246" s="1" customFormat="1" spans="6:12">
+    <row r="246" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F246" s="6"/>
       <c r="L246" s="6"/>
     </row>
-    <row r="247" s="1" customFormat="1" spans="6:12">
+    <row r="247" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F247" s="6"/>
       <c r="L247" s="6"/>
     </row>
-    <row r="248" s="1" customFormat="1" spans="6:12">
+    <row r="248" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F248" s="6"/>
       <c r="L248" s="6"/>
     </row>
-    <row r="249" s="1" customFormat="1" spans="6:12">
+    <row r="249" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F249" s="6"/>
       <c r="L249" s="6"/>
     </row>
-    <row r="250" s="1" customFormat="1" spans="6:12">
+    <row r="250" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F250" s="6"/>
       <c r="L250" s="6"/>
     </row>
-    <row r="251" s="1" customFormat="1" spans="6:12">
+    <row r="251" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F251" s="6"/>
       <c r="L251" s="6"/>
     </row>
-    <row r="252" s="1" customFormat="1" spans="6:12">
+    <row r="252" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F252" s="6"/>
       <c r="L252" s="6"/>
     </row>
-    <row r="253" s="1" customFormat="1" spans="6:12">
+    <row r="253" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F253" s="6"/>
       <c r="L253" s="6"/>
     </row>
-    <row r="254" s="1" customFormat="1" spans="6:12">
+    <row r="254" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F254" s="6"/>
       <c r="L254" s="6"/>
     </row>
-    <row r="255" s="1" customFormat="1" spans="6:12">
+    <row r="255" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F255" s="6"/>
       <c r="L255" s="6"/>
     </row>
-    <row r="256" s="1" customFormat="1" spans="6:12">
+    <row r="256" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F256" s="6"/>
       <c r="L256" s="6"/>
     </row>
-    <row r="257" s="1" customFormat="1" spans="6:12">
+    <row r="257" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F257" s="6"/>
       <c r="L257" s="6"/>
     </row>
-    <row r="258" s="1" customFormat="1" spans="6:12">
+    <row r="258" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F258" s="6"/>
       <c r="L258" s="6"/>
     </row>
-    <row r="259" s="1" customFormat="1" spans="6:12">
+    <row r="259" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F259" s="6"/>
       <c r="L259" s="6"/>
     </row>
-    <row r="260" s="1" customFormat="1" spans="6:12">
+    <row r="260" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F260" s="6"/>
       <c r="L260" s="6"/>
     </row>
-    <row r="261" s="1" customFormat="1" spans="6:12">
+    <row r="261" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F261" s="6"/>
       <c r="L261" s="6"/>
     </row>
-    <row r="262" s="1" customFormat="1" spans="6:12">
+    <row r="262" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F262" s="6"/>
       <c r="L262" s="6"/>
     </row>
-    <row r="263" s="1" customFormat="1" spans="6:12">
+    <row r="263" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F263" s="6"/>
       <c r="L263" s="6"/>
     </row>
-    <row r="264" s="1" customFormat="1" spans="6:12">
+    <row r="264" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F264" s="6"/>
       <c r="L264" s="6"/>
     </row>
-    <row r="265" s="1" customFormat="1" spans="6:12">
+    <row r="265" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F265" s="6"/>
       <c r="L265" s="6"/>
     </row>
-    <row r="266" s="1" customFormat="1" spans="6:12">
+    <row r="266" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F266" s="6"/>
       <c r="L266" s="6"/>
     </row>
-    <row r="267" s="1" customFormat="1" spans="6:12">
+    <row r="267" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F267" s="6"/>
       <c r="L267" s="6"/>
     </row>
-    <row r="268" s="1" customFormat="1" spans="6:12">
+    <row r="268" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F268" s="6"/>
       <c r="L268" s="6"/>
     </row>
-    <row r="269" s="1" customFormat="1" spans="6:12">
+    <row r="269" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F269" s="6"/>
       <c r="L269" s="6"/>
     </row>
-    <row r="270" s="1" customFormat="1" spans="6:12">
+    <row r="270" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F270" s="6"/>
       <c r="L270" s="6"/>
     </row>
-    <row r="271" s="1" customFormat="1" spans="6:12">
+    <row r="271" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F271" s="6"/>
       <c r="L271" s="6"/>
     </row>
-    <row r="272" s="1" customFormat="1" spans="6:12">
+    <row r="272" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F272" s="6"/>
       <c r="L272" s="6"/>
     </row>
-    <row r="273" s="1" customFormat="1" spans="6:12">
+    <row r="273" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F273" s="6"/>
       <c r="L273" s="6"/>
     </row>
-    <row r="274" s="1" customFormat="1" spans="6:12">
+    <row r="274" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F274" s="6"/>
       <c r="L274" s="6"/>
     </row>
-    <row r="275" s="1" customFormat="1" spans="6:12">
+    <row r="275" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F275" s="6"/>
       <c r="L275" s="6"/>
     </row>
-    <row r="276" s="1" customFormat="1" spans="6:12">
+    <row r="276" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F276" s="6"/>
       <c r="L276" s="6"/>
     </row>
-    <row r="277" s="1" customFormat="1" spans="6:12">
+    <row r="277" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F277" s="6"/>
       <c r="L277" s="6"/>
     </row>
-    <row r="278" s="1" customFormat="1" spans="6:12">
+    <row r="278" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F278" s="6"/>
       <c r="L278" s="6"/>
     </row>
-    <row r="279" s="1" customFormat="1" spans="6:12">
+    <row r="279" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F279" s="6"/>
       <c r="L279" s="6"/>
     </row>
-    <row r="280" s="1" customFormat="1" spans="6:12">
+    <row r="280" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F280" s="6"/>
       <c r="L280" s="6"/>
     </row>
-    <row r="281" s="1" customFormat="1" spans="6:12">
+    <row r="281" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F281" s="6"/>
       <c r="L281" s="6"/>
     </row>
-    <row r="282" s="1" customFormat="1" spans="6:12">
+    <row r="282" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F282" s="6"/>
       <c r="L282" s="6"/>
     </row>
-    <row r="283" s="1" customFormat="1" spans="6:12">
+    <row r="283" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F283" s="6"/>
       <c r="L283" s="6"/>
     </row>
-    <row r="284" s="1" customFormat="1" spans="6:12">
+    <row r="284" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F284" s="6"/>
       <c r="L284" s="6"/>
     </row>
-    <row r="285" s="1" customFormat="1" spans="6:12">
+    <row r="285" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F285" s="6"/>
       <c r="L285" s="6"/>
     </row>
-    <row r="286" s="1" customFormat="1" spans="6:12">
+    <row r="286" s="1" customFormat="1" ht="14.25" spans="6:12">
       <c r="F286" s="6"/>
       <c r="L286" s="6"/>
-    </row>
-    <row r="287" s="1" customFormat="1" spans="6:12">
-      <c r="F287" s="6"/>
-      <c r="L287" s="6"/>
-    </row>
-    <row r="288" s="1" customFormat="1" spans="6:12">
-      <c r="F288" s="6"/>
-      <c r="L288" s="6"/>
-    </row>
-    <row r="289" s="1" customFormat="1" spans="6:12">
-      <c r="F289" s="6"/>
-      <c r="L289" s="6"/>
-    </row>
-    <row r="290" s="1" customFormat="1" spans="6:12">
-      <c r="F290" s="6"/>
-      <c r="L290" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Revert "Merge branch 'new-dev' into WT-886-Update-DRS-issue"
This reverts commit f0de7adcfce5d91bf24b9a49bbb9c59d3a2360ad, reversing
changes made to 63e98f2c5ea73362966158d11d83c6fcfcfe9e93.
</commit_message>
<xml_diff>
--- a/src/assets/Download/CustomerMasterTemplate.xlsx
+++ b/src/assets/Download/CustomerMasterTemplate.xlsx
@@ -4,17 +4,30 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650"/>
+    <workbookView windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>CustomerGroup</t>
   </si>
@@ -52,15 +65,6 @@
     <t>PinCode</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>MSMENo</t>
   </si>
   <si>
@@ -101,15 +105,6 @@
   </si>
   <si>
     <t>831001</t>
-  </si>
-  <si>
-    <t>Jamshedpur</t>
-  </si>
-  <si>
-    <t>Jharkhand</t>
-  </si>
-  <si>
-    <t>India</t>
   </si>
   <si>
     <t>4886996885</t>
@@ -124,7 +119,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -1309,10 +1304,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R286"/>
+  <dimension ref="A1:O286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1329,16 +1324,13 @@
     <col min="10" max="10" width="13.4285714285714" style="2" customWidth="1"/>
     <col min="11" max="11" width="56" style="2" customWidth="1"/>
     <col min="12" max="12" width="10.2857142857143" style="3" customWidth="1"/>
-    <col min="13" max="13" width="13.5714285714286" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.2857142857143" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.57142857142857" style="2" customWidth="1"/>
-    <col min="16" max="16" width="13.4285714285714" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.8571428571429" style="2" customWidth="1"/>
-    <col min="18" max="18" width="7.85714285714286" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="9.14285714285714" style="2"/>
+    <col min="13" max="13" width="13.4285714285714" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.8571428571429" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7.85714285714286" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.14285714285714" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1384,70 +1376,52 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:15">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:18">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="F2" s="6">
         <v>9311555369</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="L2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="O2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="6:12">
@@ -1470,1119 +1444,1119 @@
       <c r="F7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="8" s="1" customFormat="1" spans="6:12">
       <c r="F8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="9" s="1" customFormat="1" spans="6:12">
       <c r="F9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="10" s="1" customFormat="1" spans="6:12">
       <c r="F10" s="6"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="11" s="1" customFormat="1" spans="6:12">
       <c r="F11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="12" s="1" customFormat="1" spans="6:12">
       <c r="F12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="13" s="1" customFormat="1" spans="6:12">
       <c r="F13" s="6"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="14" s="1" customFormat="1" spans="6:12">
       <c r="F14" s="6"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="15" s="1" customFormat="1" spans="6:12">
       <c r="F15" s="6"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="16" s="1" customFormat="1" spans="6:12">
       <c r="F16" s="6"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="17" s="1" customFormat="1" spans="6:12">
       <c r="F17" s="6"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="18" s="1" customFormat="1" spans="6:12">
       <c r="F18" s="6"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="19" s="1" customFormat="1" spans="6:12">
       <c r="F19" s="6"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="20" s="1" customFormat="1" spans="6:12">
       <c r="F20" s="6"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="21" s="1" customFormat="1" spans="6:12">
       <c r="F21" s="6"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="22" s="1" customFormat="1" spans="6:12">
       <c r="F22" s="6"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="23" s="1" customFormat="1" spans="6:12">
       <c r="F23" s="6"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="24" s="1" customFormat="1" spans="6:12">
       <c r="F24" s="6"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="25" s="1" customFormat="1" spans="6:12">
       <c r="F25" s="6"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="26" s="1" customFormat="1" spans="6:12">
       <c r="F26" s="6"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="27" s="1" customFormat="1" spans="6:12">
       <c r="F27" s="6"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="28" s="1" customFormat="1" spans="6:12">
       <c r="F28" s="6"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="29" s="1" customFormat="1" spans="6:12">
       <c r="F29" s="6"/>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="30" s="1" customFormat="1" spans="6:12">
       <c r="F30" s="6"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="31" s="1" customFormat="1" spans="6:12">
       <c r="F31" s="6"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="32" s="1" customFormat="1" spans="6:12">
       <c r="F32" s="6"/>
       <c r="L32" s="6"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="33" s="1" customFormat="1" spans="6:12">
       <c r="F33" s="6"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="34" s="1" customFormat="1" spans="6:12">
       <c r="F34" s="6"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="35" s="1" customFormat="1" spans="6:12">
       <c r="F35" s="6"/>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="36" s="1" customFormat="1" spans="6:12">
       <c r="F36" s="6"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="37" s="1" customFormat="1" spans="6:12">
       <c r="F37" s="6"/>
       <c r="L37" s="6"/>
     </row>
-    <row r="38" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="38" s="1" customFormat="1" spans="6:12">
       <c r="F38" s="6"/>
       <c r="L38" s="6"/>
     </row>
-    <row r="39" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="39" s="1" customFormat="1" spans="6:12">
       <c r="F39" s="6"/>
       <c r="L39" s="6"/>
     </row>
-    <row r="40" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="40" s="1" customFormat="1" spans="6:12">
       <c r="F40" s="6"/>
       <c r="L40" s="6"/>
     </row>
-    <row r="41" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="41" s="1" customFormat="1" spans="6:12">
       <c r="F41" s="6"/>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="42" s="1" customFormat="1" spans="6:12">
       <c r="F42" s="6"/>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="43" s="1" customFormat="1" spans="6:12">
       <c r="F43" s="6"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="44" s="1" customFormat="1" spans="6:12">
       <c r="F44" s="6"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="45" s="1" customFormat="1" spans="6:12">
       <c r="F45" s="6"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="46" s="1" customFormat="1" spans="6:12">
       <c r="F46" s="6"/>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="47" s="1" customFormat="1" spans="6:12">
       <c r="F47" s="6"/>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="48" s="1" customFormat="1" spans="6:12">
       <c r="F48" s="6"/>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="49" s="1" customFormat="1" spans="6:12">
       <c r="F49" s="6"/>
       <c r="L49" s="6"/>
     </row>
-    <row r="50" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="50" s="1" customFormat="1" spans="6:12">
       <c r="F50" s="6"/>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="51" s="1" customFormat="1" spans="6:12">
       <c r="F51" s="6"/>
       <c r="L51" s="6"/>
     </row>
-    <row r="52" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="52" s="1" customFormat="1" spans="6:12">
       <c r="F52" s="6"/>
       <c r="L52" s="6"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="53" s="1" customFormat="1" spans="6:12">
       <c r="F53" s="6"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="54" s="1" customFormat="1" spans="6:12">
       <c r="F54" s="6"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="55" s="1" customFormat="1" spans="6:12">
       <c r="F55" s="6"/>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="56" s="1" customFormat="1" spans="6:12">
       <c r="F56" s="6"/>
       <c r="L56" s="6"/>
     </row>
-    <row r="57" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="57" s="1" customFormat="1" spans="6:12">
       <c r="F57" s="6"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="58" s="1" customFormat="1" spans="6:12">
       <c r="F58" s="6"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="59" s="1" customFormat="1" spans="6:12">
       <c r="F59" s="6"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="60" s="1" customFormat="1" spans="6:12">
       <c r="F60" s="6"/>
       <c r="L60" s="6"/>
     </row>
-    <row r="61" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="61" s="1" customFormat="1" spans="6:12">
       <c r="F61" s="6"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="62" s="1" customFormat="1" spans="6:12">
       <c r="F62" s="6"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="63" s="1" customFormat="1" spans="6:12">
       <c r="F63" s="6"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="64" s="1" customFormat="1" spans="6:12">
       <c r="F64" s="6"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="65" s="1" customFormat="1" spans="6:12">
       <c r="F65" s="6"/>
       <c r="L65" s="6"/>
     </row>
-    <row r="66" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="66" s="1" customFormat="1" spans="6:12">
       <c r="F66" s="6"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="67" s="1" customFormat="1" spans="6:12">
       <c r="F67" s="6"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="68" s="1" customFormat="1" spans="6:12">
       <c r="F68" s="6"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="69" s="1" customFormat="1" spans="6:12">
       <c r="F69" s="6"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="70" s="1" customFormat="1" spans="6:12">
       <c r="F70" s="6"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="71" s="1" customFormat="1" spans="6:12">
       <c r="F71" s="6"/>
       <c r="L71" s="6"/>
     </row>
-    <row r="72" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="72" s="1" customFormat="1" spans="6:12">
       <c r="F72" s="6"/>
       <c r="L72" s="6"/>
     </row>
-    <row r="73" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="73" s="1" customFormat="1" spans="6:12">
       <c r="F73" s="6"/>
       <c r="L73" s="6"/>
     </row>
-    <row r="74" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="74" s="1" customFormat="1" spans="6:12">
       <c r="F74" s="6"/>
       <c r="L74" s="6"/>
     </row>
-    <row r="75" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="75" s="1" customFormat="1" spans="6:12">
       <c r="F75" s="6"/>
       <c r="L75" s="6"/>
     </row>
-    <row r="76" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="76" s="1" customFormat="1" spans="6:12">
       <c r="F76" s="6"/>
       <c r="L76" s="6"/>
     </row>
-    <row r="77" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="77" s="1" customFormat="1" spans="6:12">
       <c r="F77" s="6"/>
       <c r="L77" s="6"/>
     </row>
-    <row r="78" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="78" s="1" customFormat="1" spans="6:12">
       <c r="F78" s="6"/>
       <c r="L78" s="6"/>
     </row>
-    <row r="79" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="79" s="1" customFormat="1" spans="6:12">
       <c r="F79" s="6"/>
       <c r="L79" s="6"/>
     </row>
-    <row r="80" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="80" s="1" customFormat="1" spans="6:12">
       <c r="F80" s="6"/>
       <c r="L80" s="6"/>
     </row>
-    <row r="81" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="81" s="1" customFormat="1" spans="6:12">
       <c r="F81" s="6"/>
       <c r="L81" s="6"/>
     </row>
-    <row r="82" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="82" s="1" customFormat="1" spans="6:12">
       <c r="F82" s="6"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="83" s="1" customFormat="1" spans="6:12">
       <c r="F83" s="6"/>
       <c r="L83" s="6"/>
     </row>
-    <row r="84" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="84" s="1" customFormat="1" spans="6:12">
       <c r="F84" s="6"/>
       <c r="L84" s="6"/>
     </row>
-    <row r="85" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="85" s="1" customFormat="1" spans="6:12">
       <c r="F85" s="6"/>
       <c r="L85" s="6"/>
     </row>
-    <row r="86" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="86" s="1" customFormat="1" spans="6:12">
       <c r="F86" s="6"/>
       <c r="L86" s="6"/>
     </row>
-    <row r="87" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="87" s="1" customFormat="1" spans="6:12">
       <c r="F87" s="6"/>
       <c r="L87" s="6"/>
     </row>
-    <row r="88" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="88" s="1" customFormat="1" spans="6:12">
       <c r="F88" s="6"/>
       <c r="L88" s="6"/>
     </row>
-    <row r="89" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="89" s="1" customFormat="1" spans="6:12">
       <c r="F89" s="6"/>
       <c r="L89" s="6"/>
     </row>
-    <row r="90" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="90" s="1" customFormat="1" spans="6:12">
       <c r="F90" s="6"/>
       <c r="L90" s="6"/>
     </row>
-    <row r="91" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="91" s="1" customFormat="1" spans="6:12">
       <c r="F91" s="6"/>
       <c r="L91" s="6"/>
     </row>
-    <row r="92" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="92" s="1" customFormat="1" spans="6:12">
       <c r="F92" s="6"/>
       <c r="L92" s="6"/>
     </row>
-    <row r="93" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="93" s="1" customFormat="1" spans="6:12">
       <c r="F93" s="6"/>
       <c r="L93" s="6"/>
     </row>
-    <row r="94" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="94" s="1" customFormat="1" spans="6:12">
       <c r="F94" s="6"/>
       <c r="L94" s="6"/>
     </row>
-    <row r="95" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="95" s="1" customFormat="1" spans="6:12">
       <c r="F95" s="6"/>
       <c r="L95" s="6"/>
     </row>
-    <row r="96" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="96" s="1" customFormat="1" spans="6:12">
       <c r="F96" s="6"/>
       <c r="L96" s="6"/>
     </row>
-    <row r="97" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="97" s="1" customFormat="1" spans="6:12">
       <c r="F97" s="6"/>
       <c r="L97" s="6"/>
     </row>
-    <row r="98" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="98" s="1" customFormat="1" spans="6:12">
       <c r="F98" s="6"/>
       <c r="L98" s="6"/>
     </row>
-    <row r="99" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="99" s="1" customFormat="1" spans="6:12">
       <c r="F99" s="6"/>
       <c r="L99" s="6"/>
     </row>
-    <row r="100" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="100" s="1" customFormat="1" spans="6:12">
       <c r="F100" s="6"/>
       <c r="L100" s="6"/>
     </row>
-    <row r="101" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="101" s="1" customFormat="1" spans="6:12">
       <c r="F101" s="6"/>
       <c r="L101" s="6"/>
     </row>
-    <row r="102" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="102" s="1" customFormat="1" spans="6:12">
       <c r="F102" s="6"/>
       <c r="L102" s="6"/>
     </row>
-    <row r="103" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="103" s="1" customFormat="1" spans="6:12">
       <c r="F103" s="6"/>
       <c r="L103" s="6"/>
     </row>
-    <row r="104" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="104" s="1" customFormat="1" spans="6:12">
       <c r="F104" s="6"/>
       <c r="L104" s="6"/>
     </row>
-    <row r="105" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="105" s="1" customFormat="1" spans="6:12">
       <c r="F105" s="6"/>
       <c r="L105" s="6"/>
     </row>
-    <row r="106" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="106" s="1" customFormat="1" spans="6:12">
       <c r="F106" s="6"/>
       <c r="L106" s="6"/>
     </row>
-    <row r="107" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="107" s="1" customFormat="1" spans="6:12">
       <c r="F107" s="6"/>
       <c r="L107" s="6"/>
     </row>
-    <row r="108" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="108" s="1" customFormat="1" spans="6:12">
       <c r="F108" s="6"/>
       <c r="L108" s="6"/>
     </row>
-    <row r="109" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="109" s="1" customFormat="1" spans="6:12">
       <c r="F109" s="6"/>
       <c r="L109" s="6"/>
     </row>
-    <row r="110" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="110" s="1" customFormat="1" spans="6:12">
       <c r="F110" s="6"/>
       <c r="L110" s="6"/>
     </row>
-    <row r="111" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="111" s="1" customFormat="1" spans="6:12">
       <c r="F111" s="6"/>
       <c r="L111" s="6"/>
     </row>
-    <row r="112" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="112" s="1" customFormat="1" spans="6:12">
       <c r="F112" s="6"/>
       <c r="L112" s="6"/>
     </row>
-    <row r="113" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="113" s="1" customFormat="1" spans="6:12">
       <c r="F113" s="6"/>
       <c r="L113" s="6"/>
     </row>
-    <row r="114" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="114" s="1" customFormat="1" spans="6:12">
       <c r="F114" s="6"/>
       <c r="L114" s="6"/>
     </row>
-    <row r="115" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="115" s="1" customFormat="1" spans="6:12">
       <c r="F115" s="6"/>
       <c r="L115" s="6"/>
     </row>
-    <row r="116" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="116" s="1" customFormat="1" spans="6:12">
       <c r="F116" s="6"/>
       <c r="L116" s="6"/>
     </row>
-    <row r="117" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="117" s="1" customFormat="1" spans="6:12">
       <c r="F117" s="6"/>
       <c r="L117" s="6"/>
     </row>
-    <row r="118" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="118" s="1" customFormat="1" spans="6:12">
       <c r="F118" s="6"/>
       <c r="L118" s="6"/>
     </row>
-    <row r="119" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="119" s="1" customFormat="1" spans="6:12">
       <c r="F119" s="6"/>
       <c r="L119" s="6"/>
     </row>
-    <row r="120" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="120" s="1" customFormat="1" spans="6:12">
       <c r="F120" s="6"/>
       <c r="L120" s="6"/>
     </row>
-    <row r="121" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="121" s="1" customFormat="1" spans="6:12">
       <c r="F121" s="6"/>
       <c r="L121" s="6"/>
     </row>
-    <row r="122" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="122" s="1" customFormat="1" spans="6:12">
       <c r="F122" s="6"/>
       <c r="L122" s="6"/>
     </row>
-    <row r="123" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="123" s="1" customFormat="1" spans="6:12">
       <c r="F123" s="6"/>
       <c r="L123" s="6"/>
     </row>
-    <row r="124" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="124" s="1" customFormat="1" spans="6:12">
       <c r="F124" s="6"/>
       <c r="L124" s="6"/>
     </row>
-    <row r="125" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="125" s="1" customFormat="1" spans="6:12">
       <c r="F125" s="6"/>
       <c r="L125" s="6"/>
     </row>
-    <row r="126" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="126" s="1" customFormat="1" spans="6:12">
       <c r="F126" s="6"/>
       <c r="L126" s="6"/>
     </row>
-    <row r="127" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="127" s="1" customFormat="1" spans="6:12">
       <c r="F127" s="6"/>
       <c r="L127" s="6"/>
     </row>
-    <row r="128" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="128" s="1" customFormat="1" spans="6:12">
       <c r="F128" s="6"/>
       <c r="L128" s="6"/>
     </row>
-    <row r="129" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="129" s="1" customFormat="1" spans="6:12">
       <c r="F129" s="6"/>
       <c r="L129" s="6"/>
     </row>
-    <row r="130" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="130" s="1" customFormat="1" spans="6:12">
       <c r="F130" s="6"/>
       <c r="L130" s="6"/>
     </row>
-    <row r="131" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="131" s="1" customFormat="1" spans="6:12">
       <c r="F131" s="6"/>
       <c r="L131" s="6"/>
     </row>
-    <row r="132" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="132" s="1" customFormat="1" spans="6:12">
       <c r="F132" s="6"/>
       <c r="L132" s="6"/>
     </row>
-    <row r="133" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="133" s="1" customFormat="1" spans="6:12">
       <c r="F133" s="6"/>
       <c r="L133" s="6"/>
     </row>
-    <row r="134" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="134" s="1" customFormat="1" spans="6:12">
       <c r="F134" s="6"/>
       <c r="L134" s="6"/>
     </row>
-    <row r="135" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="135" s="1" customFormat="1" spans="6:12">
       <c r="F135" s="6"/>
       <c r="L135" s="6"/>
     </row>
-    <row r="136" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="136" s="1" customFormat="1" spans="6:12">
       <c r="F136" s="6"/>
       <c r="L136" s="6"/>
     </row>
-    <row r="137" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="137" s="1" customFormat="1" spans="6:12">
       <c r="F137" s="6"/>
       <c r="L137" s="6"/>
     </row>
-    <row r="138" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="138" s="1" customFormat="1" spans="6:12">
       <c r="F138" s="6"/>
       <c r="L138" s="6"/>
     </row>
-    <row r="139" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="139" s="1" customFormat="1" spans="6:12">
       <c r="F139" s="6"/>
       <c r="L139" s="6"/>
     </row>
-    <row r="140" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="140" s="1" customFormat="1" spans="6:12">
       <c r="F140" s="6"/>
       <c r="L140" s="6"/>
     </row>
-    <row r="141" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="141" s="1" customFormat="1" spans="6:12">
       <c r="F141" s="6"/>
       <c r="L141" s="6"/>
     </row>
-    <row r="142" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="142" s="1" customFormat="1" spans="6:12">
       <c r="F142" s="6"/>
       <c r="L142" s="6"/>
     </row>
-    <row r="143" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="143" s="1" customFormat="1" spans="6:12">
       <c r="F143" s="6"/>
       <c r="L143" s="6"/>
     </row>
-    <row r="144" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="144" s="1" customFormat="1" spans="6:12">
       <c r="F144" s="6"/>
       <c r="L144" s="6"/>
     </row>
-    <row r="145" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="145" s="1" customFormat="1" spans="6:12">
       <c r="F145" s="6"/>
       <c r="L145" s="6"/>
     </row>
-    <row r="146" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="146" s="1" customFormat="1" spans="6:12">
       <c r="F146" s="6"/>
       <c r="L146" s="6"/>
     </row>
-    <row r="147" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="147" s="1" customFormat="1" spans="6:12">
       <c r="F147" s="6"/>
       <c r="L147" s="6"/>
     </row>
-    <row r="148" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="148" s="1" customFormat="1" spans="6:12">
       <c r="F148" s="6"/>
       <c r="L148" s="6"/>
     </row>
-    <row r="149" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="149" s="1" customFormat="1" spans="6:12">
       <c r="F149" s="6"/>
       <c r="L149" s="6"/>
     </row>
-    <row r="150" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="150" s="1" customFormat="1" spans="6:12">
       <c r="F150" s="6"/>
       <c r="L150" s="6"/>
     </row>
-    <row r="151" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="151" s="1" customFormat="1" spans="6:12">
       <c r="F151" s="6"/>
       <c r="L151" s="6"/>
     </row>
-    <row r="152" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="152" s="1" customFormat="1" spans="6:12">
       <c r="F152" s="6"/>
       <c r="L152" s="6"/>
     </row>
-    <row r="153" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="153" s="1" customFormat="1" spans="6:12">
       <c r="F153" s="6"/>
       <c r="L153" s="6"/>
     </row>
-    <row r="154" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="154" s="1" customFormat="1" spans="6:12">
       <c r="F154" s="6"/>
       <c r="L154" s="6"/>
     </row>
-    <row r="155" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="155" s="1" customFormat="1" spans="6:12">
       <c r="F155" s="6"/>
       <c r="L155" s="6"/>
     </row>
-    <row r="156" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="156" s="1" customFormat="1" spans="6:12">
       <c r="F156" s="6"/>
       <c r="L156" s="6"/>
     </row>
-    <row r="157" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="157" s="1" customFormat="1" spans="6:12">
       <c r="F157" s="6"/>
       <c r="L157" s="6"/>
     </row>
-    <row r="158" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="158" s="1" customFormat="1" spans="6:12">
       <c r="F158" s="6"/>
       <c r="L158" s="6"/>
     </row>
-    <row r="159" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="159" s="1" customFormat="1" spans="6:12">
       <c r="F159" s="6"/>
       <c r="L159" s="6"/>
     </row>
-    <row r="160" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="160" s="1" customFormat="1" spans="6:12">
       <c r="F160" s="6"/>
       <c r="L160" s="6"/>
     </row>
-    <row r="161" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="161" s="1" customFormat="1" spans="6:12">
       <c r="F161" s="6"/>
       <c r="L161" s="6"/>
     </row>
-    <row r="162" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="162" s="1" customFormat="1" spans="6:12">
       <c r="F162" s="6"/>
       <c r="L162" s="6"/>
     </row>
-    <row r="163" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="163" s="1" customFormat="1" spans="6:12">
       <c r="F163" s="6"/>
       <c r="L163" s="6"/>
     </row>
-    <row r="164" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="164" s="1" customFormat="1" spans="6:12">
       <c r="F164" s="6"/>
       <c r="L164" s="6"/>
     </row>
-    <row r="165" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="165" s="1" customFormat="1" spans="6:12">
       <c r="F165" s="6"/>
       <c r="L165" s="6"/>
     </row>
-    <row r="166" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="166" s="1" customFormat="1" spans="6:12">
       <c r="F166" s="6"/>
       <c r="L166" s="6"/>
     </row>
-    <row r="167" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="167" s="1" customFormat="1" spans="6:12">
       <c r="F167" s="6"/>
       <c r="L167" s="6"/>
     </row>
-    <row r="168" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="168" s="1" customFormat="1" spans="6:12">
       <c r="F168" s="6"/>
       <c r="L168" s="6"/>
     </row>
-    <row r="169" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="169" s="1" customFormat="1" spans="6:12">
       <c r="F169" s="6"/>
       <c r="L169" s="6"/>
     </row>
-    <row r="170" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="170" s="1" customFormat="1" spans="6:12">
       <c r="F170" s="6"/>
       <c r="L170" s="6"/>
     </row>
-    <row r="171" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="171" s="1" customFormat="1" spans="6:12">
       <c r="F171" s="6"/>
       <c r="L171" s="6"/>
     </row>
-    <row r="172" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="172" s="1" customFormat="1" spans="6:12">
       <c r="F172" s="6"/>
       <c r="L172" s="6"/>
     </row>
-    <row r="173" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="173" s="1" customFormat="1" spans="6:12">
       <c r="F173" s="6"/>
       <c r="L173" s="6"/>
     </row>
-    <row r="174" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="174" s="1" customFormat="1" spans="6:12">
       <c r="F174" s="6"/>
       <c r="L174" s="6"/>
     </row>
-    <row r="175" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="175" s="1" customFormat="1" spans="6:12">
       <c r="F175" s="6"/>
       <c r="L175" s="6"/>
     </row>
-    <row r="176" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="176" s="1" customFormat="1" spans="6:12">
       <c r="F176" s="6"/>
       <c r="L176" s="6"/>
     </row>
-    <row r="177" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="177" s="1" customFormat="1" spans="6:12">
       <c r="F177" s="6"/>
       <c r="L177" s="6"/>
     </row>
-    <row r="178" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="178" s="1" customFormat="1" spans="6:12">
       <c r="F178" s="6"/>
       <c r="L178" s="6"/>
     </row>
-    <row r="179" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="179" s="1" customFormat="1" spans="6:12">
       <c r="F179" s="6"/>
       <c r="L179" s="6"/>
     </row>
-    <row r="180" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="180" s="1" customFormat="1" spans="6:12">
       <c r="F180" s="6"/>
       <c r="L180" s="6"/>
     </row>
-    <row r="181" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="181" s="1" customFormat="1" spans="6:12">
       <c r="F181" s="6"/>
       <c r="L181" s="6"/>
     </row>
-    <row r="182" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="182" s="1" customFormat="1" spans="6:12">
       <c r="F182" s="6"/>
       <c r="L182" s="6"/>
     </row>
-    <row r="183" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="183" s="1" customFormat="1" spans="6:12">
       <c r="F183" s="6"/>
       <c r="L183" s="6"/>
     </row>
-    <row r="184" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="184" s="1" customFormat="1" spans="6:12">
       <c r="F184" s="6"/>
       <c r="L184" s="6"/>
     </row>
-    <row r="185" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="185" s="1" customFormat="1" spans="6:12">
       <c r="F185" s="6"/>
       <c r="L185" s="6"/>
     </row>
-    <row r="186" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="186" s="1" customFormat="1" spans="6:12">
       <c r="F186" s="6"/>
       <c r="L186" s="6"/>
     </row>
-    <row r="187" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="187" s="1" customFormat="1" spans="6:12">
       <c r="F187" s="6"/>
       <c r="L187" s="6"/>
     </row>
-    <row r="188" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="188" s="1" customFormat="1" spans="6:12">
       <c r="F188" s="6"/>
       <c r="L188" s="6"/>
     </row>
-    <row r="189" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="189" s="1" customFormat="1" spans="6:12">
       <c r="F189" s="6"/>
       <c r="L189" s="6"/>
     </row>
-    <row r="190" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="190" s="1" customFormat="1" spans="6:12">
       <c r="F190" s="6"/>
       <c r="L190" s="6"/>
     </row>
-    <row r="191" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="191" s="1" customFormat="1" spans="6:12">
       <c r="F191" s="6"/>
       <c r="L191" s="6"/>
     </row>
-    <row r="192" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="192" s="1" customFormat="1" spans="6:12">
       <c r="F192" s="6"/>
       <c r="L192" s="6"/>
     </row>
-    <row r="193" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="193" s="1" customFormat="1" spans="6:12">
       <c r="F193" s="6"/>
       <c r="L193" s="6"/>
     </row>
-    <row r="194" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="194" s="1" customFormat="1" spans="6:12">
       <c r="F194" s="6"/>
       <c r="L194" s="6"/>
     </row>
-    <row r="195" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="195" s="1" customFormat="1" spans="6:12">
       <c r="F195" s="6"/>
       <c r="L195" s="6"/>
     </row>
-    <row r="196" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="196" s="1" customFormat="1" spans="6:12">
       <c r="F196" s="6"/>
       <c r="L196" s="6"/>
     </row>
-    <row r="197" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="197" s="1" customFormat="1" spans="6:12">
       <c r="F197" s="6"/>
       <c r="L197" s="6"/>
     </row>
-    <row r="198" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="198" s="1" customFormat="1" spans="6:12">
       <c r="F198" s="6"/>
       <c r="L198" s="6"/>
     </row>
-    <row r="199" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="199" s="1" customFormat="1" spans="6:12">
       <c r="F199" s="6"/>
       <c r="L199" s="6"/>
     </row>
-    <row r="200" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="200" s="1" customFormat="1" spans="6:12">
       <c r="F200" s="6"/>
       <c r="L200" s="6"/>
     </row>
-    <row r="201" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="201" s="1" customFormat="1" spans="6:12">
       <c r="F201" s="6"/>
       <c r="L201" s="6"/>
     </row>
-    <row r="202" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="202" s="1" customFormat="1" spans="6:12">
       <c r="F202" s="6"/>
       <c r="L202" s="6"/>
     </row>
-    <row r="203" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="203" s="1" customFormat="1" spans="6:12">
       <c r="F203" s="6"/>
       <c r="L203" s="6"/>
     </row>
-    <row r="204" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="204" s="1" customFormat="1" spans="6:12">
       <c r="F204" s="6"/>
       <c r="L204" s="6"/>
     </row>
-    <row r="205" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="205" s="1" customFormat="1" spans="6:12">
       <c r="F205" s="6"/>
       <c r="L205" s="6"/>
     </row>
-    <row r="206" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="206" s="1" customFormat="1" spans="6:12">
       <c r="F206" s="6"/>
       <c r="L206" s="6"/>
     </row>
-    <row r="207" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="207" s="1" customFormat="1" spans="6:12">
       <c r="F207" s="6"/>
       <c r="L207" s="6"/>
     </row>
-    <row r="208" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="208" s="1" customFormat="1" spans="6:12">
       <c r="F208" s="6"/>
       <c r="L208" s="6"/>
     </row>
-    <row r="209" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="209" s="1" customFormat="1" spans="6:12">
       <c r="F209" s="6"/>
       <c r="L209" s="6"/>
     </row>
-    <row r="210" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="210" s="1" customFormat="1" spans="6:12">
       <c r="F210" s="6"/>
       <c r="L210" s="6"/>
     </row>
-    <row r="211" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="211" s="1" customFormat="1" spans="6:12">
       <c r="F211" s="6"/>
       <c r="L211" s="6"/>
     </row>
-    <row r="212" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="212" s="1" customFormat="1" spans="6:12">
       <c r="F212" s="6"/>
       <c r="L212" s="6"/>
     </row>
-    <row r="213" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="213" s="1" customFormat="1" spans="6:12">
       <c r="F213" s="6"/>
       <c r="L213" s="6"/>
     </row>
-    <row r="214" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="214" s="1" customFormat="1" spans="6:12">
       <c r="F214" s="6"/>
       <c r="L214" s="6"/>
     </row>
-    <row r="215" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="215" s="1" customFormat="1" spans="6:12">
       <c r="F215" s="6"/>
       <c r="L215" s="6"/>
     </row>
-    <row r="216" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="216" s="1" customFormat="1" spans="6:12">
       <c r="F216" s="6"/>
       <c r="L216" s="6"/>
     </row>
-    <row r="217" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="217" s="1" customFormat="1" spans="6:12">
       <c r="F217" s="6"/>
       <c r="L217" s="6"/>
     </row>
-    <row r="218" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="218" s="1" customFormat="1" spans="6:12">
       <c r="F218" s="6"/>
       <c r="L218" s="6"/>
     </row>
-    <row r="219" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="219" s="1" customFormat="1" spans="6:12">
       <c r="F219" s="6"/>
       <c r="L219" s="6"/>
     </row>
-    <row r="220" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="220" s="1" customFormat="1" spans="6:12">
       <c r="F220" s="6"/>
       <c r="L220" s="6"/>
     </row>
-    <row r="221" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="221" s="1" customFormat="1" spans="6:12">
       <c r="F221" s="6"/>
       <c r="L221" s="6"/>
     </row>
-    <row r="222" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="222" s="1" customFormat="1" spans="6:12">
       <c r="F222" s="6"/>
       <c r="L222" s="6"/>
     </row>
-    <row r="223" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="223" s="1" customFormat="1" spans="6:12">
       <c r="F223" s="6"/>
       <c r="L223" s="6"/>
     </row>
-    <row r="224" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="224" s="1" customFormat="1" spans="6:12">
       <c r="F224" s="6"/>
       <c r="L224" s="6"/>
     </row>
-    <row r="225" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="225" s="1" customFormat="1" spans="6:12">
       <c r="F225" s="6"/>
       <c r="L225" s="6"/>
     </row>
-    <row r="226" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="226" s="1" customFormat="1" spans="6:12">
       <c r="F226" s="6"/>
       <c r="L226" s="6"/>
     </row>
-    <row r="227" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="227" s="1" customFormat="1" spans="6:12">
       <c r="F227" s="6"/>
       <c r="L227" s="6"/>
     </row>
-    <row r="228" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="228" s="1" customFormat="1" spans="6:12">
       <c r="F228" s="6"/>
       <c r="L228" s="6"/>
     </row>
-    <row r="229" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="229" s="1" customFormat="1" spans="6:12">
       <c r="F229" s="6"/>
       <c r="L229" s="6"/>
     </row>
-    <row r="230" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="230" s="1" customFormat="1" spans="6:12">
       <c r="F230" s="6"/>
       <c r="L230" s="6"/>
     </row>
-    <row r="231" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="231" s="1" customFormat="1" spans="6:12">
       <c r="F231" s="6"/>
       <c r="L231" s="6"/>
     </row>
-    <row r="232" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="232" s="1" customFormat="1" spans="6:12">
       <c r="F232" s="6"/>
       <c r="L232" s="6"/>
     </row>
-    <row r="233" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="233" s="1" customFormat="1" spans="6:12">
       <c r="F233" s="6"/>
       <c r="L233" s="6"/>
     </row>
-    <row r="234" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="234" s="1" customFormat="1" spans="6:12">
       <c r="F234" s="6"/>
       <c r="L234" s="6"/>
     </row>
-    <row r="235" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="235" s="1" customFormat="1" spans="6:12">
       <c r="F235" s="6"/>
       <c r="L235" s="6"/>
     </row>
-    <row r="236" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="236" s="1" customFormat="1" spans="6:12">
       <c r="F236" s="6"/>
       <c r="L236" s="6"/>
     </row>
-    <row r="237" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="237" s="1" customFormat="1" spans="6:12">
       <c r="F237" s="6"/>
       <c r="L237" s="6"/>
     </row>
-    <row r="238" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="238" s="1" customFormat="1" spans="6:12">
       <c r="F238" s="6"/>
       <c r="L238" s="6"/>
     </row>
-    <row r="239" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="239" s="1" customFormat="1" spans="6:12">
       <c r="F239" s="6"/>
       <c r="L239" s="6"/>
     </row>
-    <row r="240" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="240" s="1" customFormat="1" spans="6:12">
       <c r="F240" s="6"/>
       <c r="L240" s="6"/>
     </row>
-    <row r="241" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="241" s="1" customFormat="1" spans="6:12">
       <c r="F241" s="6"/>
       <c r="L241" s="6"/>
     </row>
-    <row r="242" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="242" s="1" customFormat="1" spans="6:12">
       <c r="F242" s="6"/>
       <c r="L242" s="6"/>
     </row>
-    <row r="243" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="243" s="1" customFormat="1" spans="6:12">
       <c r="F243" s="6"/>
       <c r="L243" s="6"/>
     </row>
-    <row r="244" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="244" s="1" customFormat="1" spans="6:12">
       <c r="F244" s="6"/>
       <c r="L244" s="6"/>
     </row>
-    <row r="245" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="245" s="1" customFormat="1" spans="6:12">
       <c r="F245" s="6"/>
       <c r="L245" s="6"/>
     </row>
-    <row r="246" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="246" s="1" customFormat="1" spans="6:12">
       <c r="F246" s="6"/>
       <c r="L246" s="6"/>
     </row>
-    <row r="247" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="247" s="1" customFormat="1" spans="6:12">
       <c r="F247" s="6"/>
       <c r="L247" s="6"/>
     </row>
-    <row r="248" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="248" s="1" customFormat="1" spans="6:12">
       <c r="F248" s="6"/>
       <c r="L248" s="6"/>
     </row>
-    <row r="249" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="249" s="1" customFormat="1" spans="6:12">
       <c r="F249" s="6"/>
       <c r="L249" s="6"/>
     </row>
-    <row r="250" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="250" s="1" customFormat="1" spans="6:12">
       <c r="F250" s="6"/>
       <c r="L250" s="6"/>
     </row>
-    <row r="251" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="251" s="1" customFormat="1" spans="6:12">
       <c r="F251" s="6"/>
       <c r="L251" s="6"/>
     </row>
-    <row r="252" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="252" s="1" customFormat="1" spans="6:12">
       <c r="F252" s="6"/>
       <c r="L252" s="6"/>
     </row>
-    <row r="253" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="253" s="1" customFormat="1" spans="6:12">
       <c r="F253" s="6"/>
       <c r="L253" s="6"/>
     </row>
-    <row r="254" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="254" s="1" customFormat="1" spans="6:12">
       <c r="F254" s="6"/>
       <c r="L254" s="6"/>
     </row>
-    <row r="255" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="255" s="1" customFormat="1" spans="6:12">
       <c r="F255" s="6"/>
       <c r="L255" s="6"/>
     </row>
-    <row r="256" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="256" s="1" customFormat="1" spans="6:12">
       <c r="F256" s="6"/>
       <c r="L256" s="6"/>
     </row>
-    <row r="257" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="257" s="1" customFormat="1" spans="6:12">
       <c r="F257" s="6"/>
       <c r="L257" s="6"/>
     </row>
-    <row r="258" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="258" s="1" customFormat="1" spans="6:12">
       <c r="F258" s="6"/>
       <c r="L258" s="6"/>
     </row>
-    <row r="259" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="259" s="1" customFormat="1" spans="6:12">
       <c r="F259" s="6"/>
       <c r="L259" s="6"/>
     </row>
-    <row r="260" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="260" s="1" customFormat="1" spans="6:12">
       <c r="F260" s="6"/>
       <c r="L260" s="6"/>
     </row>
-    <row r="261" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="261" s="1" customFormat="1" spans="6:12">
       <c r="F261" s="6"/>
       <c r="L261" s="6"/>
     </row>
-    <row r="262" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="262" s="1" customFormat="1" spans="6:12">
       <c r="F262" s="6"/>
       <c r="L262" s="6"/>
     </row>
-    <row r="263" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="263" s="1" customFormat="1" spans="6:12">
       <c r="F263" s="6"/>
       <c r="L263" s="6"/>
     </row>
-    <row r="264" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="264" s="1" customFormat="1" spans="6:12">
       <c r="F264" s="6"/>
       <c r="L264" s="6"/>
     </row>
-    <row r="265" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="265" s="1" customFormat="1" spans="6:12">
       <c r="F265" s="6"/>
       <c r="L265" s="6"/>
     </row>
-    <row r="266" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="266" s="1" customFormat="1" spans="6:12">
       <c r="F266" s="6"/>
       <c r="L266" s="6"/>
     </row>
-    <row r="267" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="267" s="1" customFormat="1" spans="6:12">
       <c r="F267" s="6"/>
       <c r="L267" s="6"/>
     </row>
-    <row r="268" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="268" s="1" customFormat="1" spans="6:12">
       <c r="F268" s="6"/>
       <c r="L268" s="6"/>
     </row>
-    <row r="269" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="269" s="1" customFormat="1" spans="6:12">
       <c r="F269" s="6"/>
       <c r="L269" s="6"/>
     </row>
-    <row r="270" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="270" s="1" customFormat="1" spans="6:12">
       <c r="F270" s="6"/>
       <c r="L270" s="6"/>
     </row>
-    <row r="271" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="271" s="1" customFormat="1" spans="6:12">
       <c r="F271" s="6"/>
       <c r="L271" s="6"/>
     </row>
-    <row r="272" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="272" s="1" customFormat="1" spans="6:12">
       <c r="F272" s="6"/>
       <c r="L272" s="6"/>
     </row>
-    <row r="273" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="273" s="1" customFormat="1" spans="6:12">
       <c r="F273" s="6"/>
       <c r="L273" s="6"/>
     </row>
-    <row r="274" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="274" s="1" customFormat="1" spans="6:12">
       <c r="F274" s="6"/>
       <c r="L274" s="6"/>
     </row>
-    <row r="275" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="275" s="1" customFormat="1" spans="6:12">
       <c r="F275" s="6"/>
       <c r="L275" s="6"/>
     </row>
-    <row r="276" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="276" s="1" customFormat="1" spans="6:12">
       <c r="F276" s="6"/>
       <c r="L276" s="6"/>
     </row>
-    <row r="277" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="277" s="1" customFormat="1" spans="6:12">
       <c r="F277" s="6"/>
       <c r="L277" s="6"/>
     </row>
-    <row r="278" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="278" s="1" customFormat="1" spans="6:12">
       <c r="F278" s="6"/>
       <c r="L278" s="6"/>
     </row>
-    <row r="279" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="279" s="1" customFormat="1" spans="6:12">
       <c r="F279" s="6"/>
       <c r="L279" s="6"/>
     </row>
-    <row r="280" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="280" s="1" customFormat="1" spans="6:12">
       <c r="F280" s="6"/>
       <c r="L280" s="6"/>
     </row>
-    <row r="281" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="281" s="1" customFormat="1" spans="6:12">
       <c r="F281" s="6"/>
       <c r="L281" s="6"/>
     </row>
-    <row r="282" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="282" s="1" customFormat="1" spans="6:12">
       <c r="F282" s="6"/>
       <c r="L282" s="6"/>
     </row>
-    <row r="283" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="283" s="1" customFormat="1" spans="6:12">
       <c r="F283" s="6"/>
       <c r="L283" s="6"/>
     </row>
-    <row r="284" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="284" s="1" customFormat="1" spans="6:12">
       <c r="F284" s="6"/>
       <c r="L284" s="6"/>
     </row>
-    <row r="285" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="285" s="1" customFormat="1" spans="6:12">
       <c r="F285" s="6"/>
       <c r="L285" s="6"/>
     </row>
-    <row r="286" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="286" s="1" customFormat="1" spans="6:12">
       <c r="F286" s="6"/>
       <c r="L286" s="6"/>
     </row>

</xml_diff>

<commit_message>
commit regarding to new patch Update
</commit_message>
<xml_diff>
--- a/src/assets/Download/CustomerMasterTemplate.xlsx
+++ b/src/assets/Download/CustomerMasterTemplate.xlsx
@@ -4,17 +4,30 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650"/>
+    <workbookView windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>CustomerGroup</t>
   </si>
@@ -52,15 +65,6 @@
     <t>PinCode</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>MSMENo</t>
   </si>
   <si>
@@ -101,15 +105,6 @@
   </si>
   <si>
     <t>831001</t>
-  </si>
-  <si>
-    <t>Jamshedpur</t>
-  </si>
-  <si>
-    <t>Jharkhand</t>
-  </si>
-  <si>
-    <t>India</t>
   </si>
   <si>
     <t>4886996885</t>
@@ -124,7 +119,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -1309,10 +1304,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R286"/>
+  <dimension ref="A1:O286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1329,16 +1324,13 @@
     <col min="10" max="10" width="13.4285714285714" style="2" customWidth="1"/>
     <col min="11" max="11" width="56" style="2" customWidth="1"/>
     <col min="12" max="12" width="10.2857142857143" style="3" customWidth="1"/>
-    <col min="13" max="13" width="13.5714285714286" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.2857142857143" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.57142857142857" style="2" customWidth="1"/>
-    <col min="16" max="16" width="13.4285714285714" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.8571428571429" style="2" customWidth="1"/>
-    <col min="18" max="18" width="7.85714285714286" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="9.14285714285714" style="2"/>
+    <col min="13" max="13" width="13.4285714285714" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.8571428571429" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7.85714285714286" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.14285714285714" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1384,70 +1376,52 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:15">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:18">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="F2" s="6">
         <v>9311555369</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="L2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="O2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="6:12">
@@ -1470,1119 +1444,1119 @@
       <c r="F7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="8" s="1" customFormat="1" spans="6:12">
       <c r="F8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="9" s="1" customFormat="1" spans="6:12">
       <c r="F9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="10" s="1" customFormat="1" spans="6:12">
       <c r="F10" s="6"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="11" s="1" customFormat="1" spans="6:12">
       <c r="F11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="12" s="1" customFormat="1" spans="6:12">
       <c r="F12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="13" s="1" customFormat="1" spans="6:12">
       <c r="F13" s="6"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="14" s="1" customFormat="1" spans="6:12">
       <c r="F14" s="6"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="15" s="1" customFormat="1" spans="6:12">
       <c r="F15" s="6"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="16" s="1" customFormat="1" spans="6:12">
       <c r="F16" s="6"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="17" s="1" customFormat="1" spans="6:12">
       <c r="F17" s="6"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="18" s="1" customFormat="1" spans="6:12">
       <c r="F18" s="6"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="19" s="1" customFormat="1" spans="6:12">
       <c r="F19" s="6"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="20" s="1" customFormat="1" spans="6:12">
       <c r="F20" s="6"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="21" s="1" customFormat="1" spans="6:12">
       <c r="F21" s="6"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="22" s="1" customFormat="1" spans="6:12">
       <c r="F22" s="6"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="23" s="1" customFormat="1" spans="6:12">
       <c r="F23" s="6"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="24" s="1" customFormat="1" spans="6:12">
       <c r="F24" s="6"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="25" s="1" customFormat="1" spans="6:12">
       <c r="F25" s="6"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="26" s="1" customFormat="1" spans="6:12">
       <c r="F26" s="6"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="27" s="1" customFormat="1" spans="6:12">
       <c r="F27" s="6"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="28" s="1" customFormat="1" spans="6:12">
       <c r="F28" s="6"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="29" s="1" customFormat="1" spans="6:12">
       <c r="F29" s="6"/>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="30" s="1" customFormat="1" spans="6:12">
       <c r="F30" s="6"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="31" s="1" customFormat="1" spans="6:12">
       <c r="F31" s="6"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="32" s="1" customFormat="1" spans="6:12">
       <c r="F32" s="6"/>
       <c r="L32" s="6"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="33" s="1" customFormat="1" spans="6:12">
       <c r="F33" s="6"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="34" s="1" customFormat="1" spans="6:12">
       <c r="F34" s="6"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="35" s="1" customFormat="1" spans="6:12">
       <c r="F35" s="6"/>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="36" s="1" customFormat="1" spans="6:12">
       <c r="F36" s="6"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="37" s="1" customFormat="1" spans="6:12">
       <c r="F37" s="6"/>
       <c r="L37" s="6"/>
     </row>
-    <row r="38" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="38" s="1" customFormat="1" spans="6:12">
       <c r="F38" s="6"/>
       <c r="L38" s="6"/>
     </row>
-    <row r="39" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="39" s="1" customFormat="1" spans="6:12">
       <c r="F39" s="6"/>
       <c r="L39" s="6"/>
     </row>
-    <row r="40" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="40" s="1" customFormat="1" spans="6:12">
       <c r="F40" s="6"/>
       <c r="L40" s="6"/>
     </row>
-    <row r="41" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="41" s="1" customFormat="1" spans="6:12">
       <c r="F41" s="6"/>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="42" s="1" customFormat="1" spans="6:12">
       <c r="F42" s="6"/>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="43" s="1" customFormat="1" spans="6:12">
       <c r="F43" s="6"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="44" s="1" customFormat="1" spans="6:12">
       <c r="F44" s="6"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="45" s="1" customFormat="1" spans="6:12">
       <c r="F45" s="6"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="46" s="1" customFormat="1" spans="6:12">
       <c r="F46" s="6"/>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="47" s="1" customFormat="1" spans="6:12">
       <c r="F47" s="6"/>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="48" s="1" customFormat="1" spans="6:12">
       <c r="F48" s="6"/>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="49" s="1" customFormat="1" spans="6:12">
       <c r="F49" s="6"/>
       <c r="L49" s="6"/>
     </row>
-    <row r="50" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="50" s="1" customFormat="1" spans="6:12">
       <c r="F50" s="6"/>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="51" s="1" customFormat="1" spans="6:12">
       <c r="F51" s="6"/>
       <c r="L51" s="6"/>
     </row>
-    <row r="52" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="52" s="1" customFormat="1" spans="6:12">
       <c r="F52" s="6"/>
       <c r="L52" s="6"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="53" s="1" customFormat="1" spans="6:12">
       <c r="F53" s="6"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="54" s="1" customFormat="1" spans="6:12">
       <c r="F54" s="6"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="55" s="1" customFormat="1" spans="6:12">
       <c r="F55" s="6"/>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="56" s="1" customFormat="1" spans="6:12">
       <c r="F56" s="6"/>
       <c r="L56" s="6"/>
     </row>
-    <row r="57" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="57" s="1" customFormat="1" spans="6:12">
       <c r="F57" s="6"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="58" s="1" customFormat="1" spans="6:12">
       <c r="F58" s="6"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="59" s="1" customFormat="1" spans="6:12">
       <c r="F59" s="6"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="60" s="1" customFormat="1" spans="6:12">
       <c r="F60" s="6"/>
       <c r="L60" s="6"/>
     </row>
-    <row r="61" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="61" s="1" customFormat="1" spans="6:12">
       <c r="F61" s="6"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="62" s="1" customFormat="1" spans="6:12">
       <c r="F62" s="6"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="63" s="1" customFormat="1" spans="6:12">
       <c r="F63" s="6"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="64" s="1" customFormat="1" spans="6:12">
       <c r="F64" s="6"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="65" s="1" customFormat="1" spans="6:12">
       <c r="F65" s="6"/>
       <c r="L65" s="6"/>
     </row>
-    <row r="66" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="66" s="1" customFormat="1" spans="6:12">
       <c r="F66" s="6"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="67" s="1" customFormat="1" spans="6:12">
       <c r="F67" s="6"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="68" s="1" customFormat="1" spans="6:12">
       <c r="F68" s="6"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="69" s="1" customFormat="1" spans="6:12">
       <c r="F69" s="6"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="70" s="1" customFormat="1" spans="6:12">
       <c r="F70" s="6"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="71" s="1" customFormat="1" spans="6:12">
       <c r="F71" s="6"/>
       <c r="L71" s="6"/>
     </row>
-    <row r="72" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="72" s="1" customFormat="1" spans="6:12">
       <c r="F72" s="6"/>
       <c r="L72" s="6"/>
     </row>
-    <row r="73" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="73" s="1" customFormat="1" spans="6:12">
       <c r="F73" s="6"/>
       <c r="L73" s="6"/>
     </row>
-    <row r="74" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="74" s="1" customFormat="1" spans="6:12">
       <c r="F74" s="6"/>
       <c r="L74" s="6"/>
     </row>
-    <row r="75" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="75" s="1" customFormat="1" spans="6:12">
       <c r="F75" s="6"/>
       <c r="L75" s="6"/>
     </row>
-    <row r="76" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="76" s="1" customFormat="1" spans="6:12">
       <c r="F76" s="6"/>
       <c r="L76" s="6"/>
     </row>
-    <row r="77" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="77" s="1" customFormat="1" spans="6:12">
       <c r="F77" s="6"/>
       <c r="L77" s="6"/>
     </row>
-    <row r="78" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="78" s="1" customFormat="1" spans="6:12">
       <c r="F78" s="6"/>
       <c r="L78" s="6"/>
     </row>
-    <row r="79" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="79" s="1" customFormat="1" spans="6:12">
       <c r="F79" s="6"/>
       <c r="L79" s="6"/>
     </row>
-    <row r="80" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="80" s="1" customFormat="1" spans="6:12">
       <c r="F80" s="6"/>
       <c r="L80" s="6"/>
     </row>
-    <row r="81" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="81" s="1" customFormat="1" spans="6:12">
       <c r="F81" s="6"/>
       <c r="L81" s="6"/>
     </row>
-    <row r="82" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="82" s="1" customFormat="1" spans="6:12">
       <c r="F82" s="6"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="83" s="1" customFormat="1" spans="6:12">
       <c r="F83" s="6"/>
       <c r="L83" s="6"/>
     </row>
-    <row r="84" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="84" s="1" customFormat="1" spans="6:12">
       <c r="F84" s="6"/>
       <c r="L84" s="6"/>
     </row>
-    <row r="85" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="85" s="1" customFormat="1" spans="6:12">
       <c r="F85" s="6"/>
       <c r="L85" s="6"/>
     </row>
-    <row r="86" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="86" s="1" customFormat="1" spans="6:12">
       <c r="F86" s="6"/>
       <c r="L86" s="6"/>
     </row>
-    <row r="87" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="87" s="1" customFormat="1" spans="6:12">
       <c r="F87" s="6"/>
       <c r="L87" s="6"/>
     </row>
-    <row r="88" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="88" s="1" customFormat="1" spans="6:12">
       <c r="F88" s="6"/>
       <c r="L88" s="6"/>
     </row>
-    <row r="89" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="89" s="1" customFormat="1" spans="6:12">
       <c r="F89" s="6"/>
       <c r="L89" s="6"/>
     </row>
-    <row r="90" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="90" s="1" customFormat="1" spans="6:12">
       <c r="F90" s="6"/>
       <c r="L90" s="6"/>
     </row>
-    <row r="91" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="91" s="1" customFormat="1" spans="6:12">
       <c r="F91" s="6"/>
       <c r="L91" s="6"/>
     </row>
-    <row r="92" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="92" s="1" customFormat="1" spans="6:12">
       <c r="F92" s="6"/>
       <c r="L92" s="6"/>
     </row>
-    <row r="93" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="93" s="1" customFormat="1" spans="6:12">
       <c r="F93" s="6"/>
       <c r="L93" s="6"/>
     </row>
-    <row r="94" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="94" s="1" customFormat="1" spans="6:12">
       <c r="F94" s="6"/>
       <c r="L94" s="6"/>
     </row>
-    <row r="95" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="95" s="1" customFormat="1" spans="6:12">
       <c r="F95" s="6"/>
       <c r="L95" s="6"/>
     </row>
-    <row r="96" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="96" s="1" customFormat="1" spans="6:12">
       <c r="F96" s="6"/>
       <c r="L96" s="6"/>
     </row>
-    <row r="97" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="97" s="1" customFormat="1" spans="6:12">
       <c r="F97" s="6"/>
       <c r="L97" s="6"/>
     </row>
-    <row r="98" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="98" s="1" customFormat="1" spans="6:12">
       <c r="F98" s="6"/>
       <c r="L98" s="6"/>
     </row>
-    <row r="99" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="99" s="1" customFormat="1" spans="6:12">
       <c r="F99" s="6"/>
       <c r="L99" s="6"/>
     </row>
-    <row r="100" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="100" s="1" customFormat="1" spans="6:12">
       <c r="F100" s="6"/>
       <c r="L100" s="6"/>
     </row>
-    <row r="101" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="101" s="1" customFormat="1" spans="6:12">
       <c r="F101" s="6"/>
       <c r="L101" s="6"/>
     </row>
-    <row r="102" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="102" s="1" customFormat="1" spans="6:12">
       <c r="F102" s="6"/>
       <c r="L102" s="6"/>
     </row>
-    <row r="103" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="103" s="1" customFormat="1" spans="6:12">
       <c r="F103" s="6"/>
       <c r="L103" s="6"/>
     </row>
-    <row r="104" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="104" s="1" customFormat="1" spans="6:12">
       <c r="F104" s="6"/>
       <c r="L104" s="6"/>
     </row>
-    <row r="105" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="105" s="1" customFormat="1" spans="6:12">
       <c r="F105" s="6"/>
       <c r="L105" s="6"/>
     </row>
-    <row r="106" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="106" s="1" customFormat="1" spans="6:12">
       <c r="F106" s="6"/>
       <c r="L106" s="6"/>
     </row>
-    <row r="107" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="107" s="1" customFormat="1" spans="6:12">
       <c r="F107" s="6"/>
       <c r="L107" s="6"/>
     </row>
-    <row r="108" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="108" s="1" customFormat="1" spans="6:12">
       <c r="F108" s="6"/>
       <c r="L108" s="6"/>
     </row>
-    <row r="109" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="109" s="1" customFormat="1" spans="6:12">
       <c r="F109" s="6"/>
       <c r="L109" s="6"/>
     </row>
-    <row r="110" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="110" s="1" customFormat="1" spans="6:12">
       <c r="F110" s="6"/>
       <c r="L110" s="6"/>
     </row>
-    <row r="111" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="111" s="1" customFormat="1" spans="6:12">
       <c r="F111" s="6"/>
       <c r="L111" s="6"/>
     </row>
-    <row r="112" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="112" s="1" customFormat="1" spans="6:12">
       <c r="F112" s="6"/>
       <c r="L112" s="6"/>
     </row>
-    <row r="113" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="113" s="1" customFormat="1" spans="6:12">
       <c r="F113" s="6"/>
       <c r="L113" s="6"/>
     </row>
-    <row r="114" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="114" s="1" customFormat="1" spans="6:12">
       <c r="F114" s="6"/>
       <c r="L114" s="6"/>
     </row>
-    <row r="115" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="115" s="1" customFormat="1" spans="6:12">
       <c r="F115" s="6"/>
       <c r="L115" s="6"/>
     </row>
-    <row r="116" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="116" s="1" customFormat="1" spans="6:12">
       <c r="F116" s="6"/>
       <c r="L116" s="6"/>
     </row>
-    <row r="117" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="117" s="1" customFormat="1" spans="6:12">
       <c r="F117" s="6"/>
       <c r="L117" s="6"/>
     </row>
-    <row r="118" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="118" s="1" customFormat="1" spans="6:12">
       <c r="F118" s="6"/>
       <c r="L118" s="6"/>
     </row>
-    <row r="119" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="119" s="1" customFormat="1" spans="6:12">
       <c r="F119" s="6"/>
       <c r="L119" s="6"/>
     </row>
-    <row r="120" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="120" s="1" customFormat="1" spans="6:12">
       <c r="F120" s="6"/>
       <c r="L120" s="6"/>
     </row>
-    <row r="121" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="121" s="1" customFormat="1" spans="6:12">
       <c r="F121" s="6"/>
       <c r="L121" s="6"/>
     </row>
-    <row r="122" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="122" s="1" customFormat="1" spans="6:12">
       <c r="F122" s="6"/>
       <c r="L122" s="6"/>
     </row>
-    <row r="123" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="123" s="1" customFormat="1" spans="6:12">
       <c r="F123" s="6"/>
       <c r="L123" s="6"/>
     </row>
-    <row r="124" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="124" s="1" customFormat="1" spans="6:12">
       <c r="F124" s="6"/>
       <c r="L124" s="6"/>
     </row>
-    <row r="125" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="125" s="1" customFormat="1" spans="6:12">
       <c r="F125" s="6"/>
       <c r="L125" s="6"/>
     </row>
-    <row r="126" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="126" s="1" customFormat="1" spans="6:12">
       <c r="F126" s="6"/>
       <c r="L126" s="6"/>
     </row>
-    <row r="127" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="127" s="1" customFormat="1" spans="6:12">
       <c r="F127" s="6"/>
       <c r="L127" s="6"/>
     </row>
-    <row r="128" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="128" s="1" customFormat="1" spans="6:12">
       <c r="F128" s="6"/>
       <c r="L128" s="6"/>
     </row>
-    <row r="129" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="129" s="1" customFormat="1" spans="6:12">
       <c r="F129" s="6"/>
       <c r="L129" s="6"/>
     </row>
-    <row r="130" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="130" s="1" customFormat="1" spans="6:12">
       <c r="F130" s="6"/>
       <c r="L130" s="6"/>
     </row>
-    <row r="131" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="131" s="1" customFormat="1" spans="6:12">
       <c r="F131" s="6"/>
       <c r="L131" s="6"/>
     </row>
-    <row r="132" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="132" s="1" customFormat="1" spans="6:12">
       <c r="F132" s="6"/>
       <c r="L132" s="6"/>
     </row>
-    <row r="133" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="133" s="1" customFormat="1" spans="6:12">
       <c r="F133" s="6"/>
       <c r="L133" s="6"/>
     </row>
-    <row r="134" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="134" s="1" customFormat="1" spans="6:12">
       <c r="F134" s="6"/>
       <c r="L134" s="6"/>
     </row>
-    <row r="135" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="135" s="1" customFormat="1" spans="6:12">
       <c r="F135" s="6"/>
       <c r="L135" s="6"/>
     </row>
-    <row r="136" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="136" s="1" customFormat="1" spans="6:12">
       <c r="F136" s="6"/>
       <c r="L136" s="6"/>
     </row>
-    <row r="137" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="137" s="1" customFormat="1" spans="6:12">
       <c r="F137" s="6"/>
       <c r="L137" s="6"/>
     </row>
-    <row r="138" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="138" s="1" customFormat="1" spans="6:12">
       <c r="F138" s="6"/>
       <c r="L138" s="6"/>
     </row>
-    <row r="139" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="139" s="1" customFormat="1" spans="6:12">
       <c r="F139" s="6"/>
       <c r="L139" s="6"/>
     </row>
-    <row r="140" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="140" s="1" customFormat="1" spans="6:12">
       <c r="F140" s="6"/>
       <c r="L140" s="6"/>
     </row>
-    <row r="141" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="141" s="1" customFormat="1" spans="6:12">
       <c r="F141" s="6"/>
       <c r="L141" s="6"/>
     </row>
-    <row r="142" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="142" s="1" customFormat="1" spans="6:12">
       <c r="F142" s="6"/>
       <c r="L142" s="6"/>
     </row>
-    <row r="143" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="143" s="1" customFormat="1" spans="6:12">
       <c r="F143" s="6"/>
       <c r="L143" s="6"/>
     </row>
-    <row r="144" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="144" s="1" customFormat="1" spans="6:12">
       <c r="F144" s="6"/>
       <c r="L144" s="6"/>
     </row>
-    <row r="145" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="145" s="1" customFormat="1" spans="6:12">
       <c r="F145" s="6"/>
       <c r="L145" s="6"/>
     </row>
-    <row r="146" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="146" s="1" customFormat="1" spans="6:12">
       <c r="F146" s="6"/>
       <c r="L146" s="6"/>
     </row>
-    <row r="147" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="147" s="1" customFormat="1" spans="6:12">
       <c r="F147" s="6"/>
       <c r="L147" s="6"/>
     </row>
-    <row r="148" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="148" s="1" customFormat="1" spans="6:12">
       <c r="F148" s="6"/>
       <c r="L148" s="6"/>
     </row>
-    <row r="149" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="149" s="1" customFormat="1" spans="6:12">
       <c r="F149" s="6"/>
       <c r="L149" s="6"/>
     </row>
-    <row r="150" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="150" s="1" customFormat="1" spans="6:12">
       <c r="F150" s="6"/>
       <c r="L150" s="6"/>
     </row>
-    <row r="151" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="151" s="1" customFormat="1" spans="6:12">
       <c r="F151" s="6"/>
       <c r="L151" s="6"/>
     </row>
-    <row r="152" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="152" s="1" customFormat="1" spans="6:12">
       <c r="F152" s="6"/>
       <c r="L152" s="6"/>
     </row>
-    <row r="153" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="153" s="1" customFormat="1" spans="6:12">
       <c r="F153" s="6"/>
       <c r="L153" s="6"/>
     </row>
-    <row r="154" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="154" s="1" customFormat="1" spans="6:12">
       <c r="F154" s="6"/>
       <c r="L154" s="6"/>
     </row>
-    <row r="155" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="155" s="1" customFormat="1" spans="6:12">
       <c r="F155" s="6"/>
       <c r="L155" s="6"/>
     </row>
-    <row r="156" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="156" s="1" customFormat="1" spans="6:12">
       <c r="F156" s="6"/>
       <c r="L156" s="6"/>
     </row>
-    <row r="157" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="157" s="1" customFormat="1" spans="6:12">
       <c r="F157" s="6"/>
       <c r="L157" s="6"/>
     </row>
-    <row r="158" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="158" s="1" customFormat="1" spans="6:12">
       <c r="F158" s="6"/>
       <c r="L158" s="6"/>
     </row>
-    <row r="159" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="159" s="1" customFormat="1" spans="6:12">
       <c r="F159" s="6"/>
       <c r="L159" s="6"/>
     </row>
-    <row r="160" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="160" s="1" customFormat="1" spans="6:12">
       <c r="F160" s="6"/>
       <c r="L160" s="6"/>
     </row>
-    <row r="161" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="161" s="1" customFormat="1" spans="6:12">
       <c r="F161" s="6"/>
       <c r="L161" s="6"/>
     </row>
-    <row r="162" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="162" s="1" customFormat="1" spans="6:12">
       <c r="F162" s="6"/>
       <c r="L162" s="6"/>
     </row>
-    <row r="163" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="163" s="1" customFormat="1" spans="6:12">
       <c r="F163" s="6"/>
       <c r="L163" s="6"/>
     </row>
-    <row r="164" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="164" s="1" customFormat="1" spans="6:12">
       <c r="F164" s="6"/>
       <c r="L164" s="6"/>
     </row>
-    <row r="165" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="165" s="1" customFormat="1" spans="6:12">
       <c r="F165" s="6"/>
       <c r="L165" s="6"/>
     </row>
-    <row r="166" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="166" s="1" customFormat="1" spans="6:12">
       <c r="F166" s="6"/>
       <c r="L166" s="6"/>
     </row>
-    <row r="167" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="167" s="1" customFormat="1" spans="6:12">
       <c r="F167" s="6"/>
       <c r="L167" s="6"/>
     </row>
-    <row r="168" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="168" s="1" customFormat="1" spans="6:12">
       <c r="F168" s="6"/>
       <c r="L168" s="6"/>
     </row>
-    <row r="169" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="169" s="1" customFormat="1" spans="6:12">
       <c r="F169" s="6"/>
       <c r="L169" s="6"/>
     </row>
-    <row r="170" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="170" s="1" customFormat="1" spans="6:12">
       <c r="F170" s="6"/>
       <c r="L170" s="6"/>
     </row>
-    <row r="171" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="171" s="1" customFormat="1" spans="6:12">
       <c r="F171" s="6"/>
       <c r="L171" s="6"/>
     </row>
-    <row r="172" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="172" s="1" customFormat="1" spans="6:12">
       <c r="F172" s="6"/>
       <c r="L172" s="6"/>
     </row>
-    <row r="173" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="173" s="1" customFormat="1" spans="6:12">
       <c r="F173" s="6"/>
       <c r="L173" s="6"/>
     </row>
-    <row r="174" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="174" s="1" customFormat="1" spans="6:12">
       <c r="F174" s="6"/>
       <c r="L174" s="6"/>
     </row>
-    <row r="175" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="175" s="1" customFormat="1" spans="6:12">
       <c r="F175" s="6"/>
       <c r="L175" s="6"/>
     </row>
-    <row r="176" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="176" s="1" customFormat="1" spans="6:12">
       <c r="F176" s="6"/>
       <c r="L176" s="6"/>
     </row>
-    <row r="177" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="177" s="1" customFormat="1" spans="6:12">
       <c r="F177" s="6"/>
       <c r="L177" s="6"/>
     </row>
-    <row r="178" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="178" s="1" customFormat="1" spans="6:12">
       <c r="F178" s="6"/>
       <c r="L178" s="6"/>
     </row>
-    <row r="179" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="179" s="1" customFormat="1" spans="6:12">
       <c r="F179" s="6"/>
       <c r="L179" s="6"/>
     </row>
-    <row r="180" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="180" s="1" customFormat="1" spans="6:12">
       <c r="F180" s="6"/>
       <c r="L180" s="6"/>
     </row>
-    <row r="181" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="181" s="1" customFormat="1" spans="6:12">
       <c r="F181" s="6"/>
       <c r="L181" s="6"/>
     </row>
-    <row r="182" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="182" s="1" customFormat="1" spans="6:12">
       <c r="F182" s="6"/>
       <c r="L182" s="6"/>
     </row>
-    <row r="183" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="183" s="1" customFormat="1" spans="6:12">
       <c r="F183" s="6"/>
       <c r="L183" s="6"/>
     </row>
-    <row r="184" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="184" s="1" customFormat="1" spans="6:12">
       <c r="F184" s="6"/>
       <c r="L184" s="6"/>
     </row>
-    <row r="185" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="185" s="1" customFormat="1" spans="6:12">
       <c r="F185" s="6"/>
       <c r="L185" s="6"/>
     </row>
-    <row r="186" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="186" s="1" customFormat="1" spans="6:12">
       <c r="F186" s="6"/>
       <c r="L186" s="6"/>
     </row>
-    <row r="187" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="187" s="1" customFormat="1" spans="6:12">
       <c r="F187" s="6"/>
       <c r="L187" s="6"/>
     </row>
-    <row r="188" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="188" s="1" customFormat="1" spans="6:12">
       <c r="F188" s="6"/>
       <c r="L188" s="6"/>
     </row>
-    <row r="189" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="189" s="1" customFormat="1" spans="6:12">
       <c r="F189" s="6"/>
       <c r="L189" s="6"/>
     </row>
-    <row r="190" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="190" s="1" customFormat="1" spans="6:12">
       <c r="F190" s="6"/>
       <c r="L190" s="6"/>
     </row>
-    <row r="191" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="191" s="1" customFormat="1" spans="6:12">
       <c r="F191" s="6"/>
       <c r="L191" s="6"/>
     </row>
-    <row r="192" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="192" s="1" customFormat="1" spans="6:12">
       <c r="F192" s="6"/>
       <c r="L192" s="6"/>
     </row>
-    <row r="193" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="193" s="1" customFormat="1" spans="6:12">
       <c r="F193" s="6"/>
       <c r="L193" s="6"/>
     </row>
-    <row r="194" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="194" s="1" customFormat="1" spans="6:12">
       <c r="F194" s="6"/>
       <c r="L194" s="6"/>
     </row>
-    <row r="195" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="195" s="1" customFormat="1" spans="6:12">
       <c r="F195" s="6"/>
       <c r="L195" s="6"/>
     </row>
-    <row r="196" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="196" s="1" customFormat="1" spans="6:12">
       <c r="F196" s="6"/>
       <c r="L196" s="6"/>
     </row>
-    <row r="197" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="197" s="1" customFormat="1" spans="6:12">
       <c r="F197" s="6"/>
       <c r="L197" s="6"/>
     </row>
-    <row r="198" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="198" s="1" customFormat="1" spans="6:12">
       <c r="F198" s="6"/>
       <c r="L198" s="6"/>
     </row>
-    <row r="199" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="199" s="1" customFormat="1" spans="6:12">
       <c r="F199" s="6"/>
       <c r="L199" s="6"/>
     </row>
-    <row r="200" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="200" s="1" customFormat="1" spans="6:12">
       <c r="F200" s="6"/>
       <c r="L200" s="6"/>
     </row>
-    <row r="201" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="201" s="1" customFormat="1" spans="6:12">
       <c r="F201" s="6"/>
       <c r="L201" s="6"/>
     </row>
-    <row r="202" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="202" s="1" customFormat="1" spans="6:12">
       <c r="F202" s="6"/>
       <c r="L202" s="6"/>
     </row>
-    <row r="203" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="203" s="1" customFormat="1" spans="6:12">
       <c r="F203" s="6"/>
       <c r="L203" s="6"/>
     </row>
-    <row r="204" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="204" s="1" customFormat="1" spans="6:12">
       <c r="F204" s="6"/>
       <c r="L204" s="6"/>
     </row>
-    <row r="205" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="205" s="1" customFormat="1" spans="6:12">
       <c r="F205" s="6"/>
       <c r="L205" s="6"/>
     </row>
-    <row r="206" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="206" s="1" customFormat="1" spans="6:12">
       <c r="F206" s="6"/>
       <c r="L206" s="6"/>
     </row>
-    <row r="207" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="207" s="1" customFormat="1" spans="6:12">
       <c r="F207" s="6"/>
       <c r="L207" s="6"/>
     </row>
-    <row r="208" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="208" s="1" customFormat="1" spans="6:12">
       <c r="F208" s="6"/>
       <c r="L208" s="6"/>
     </row>
-    <row r="209" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="209" s="1" customFormat="1" spans="6:12">
       <c r="F209" s="6"/>
       <c r="L209" s="6"/>
     </row>
-    <row r="210" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="210" s="1" customFormat="1" spans="6:12">
       <c r="F210" s="6"/>
       <c r="L210" s="6"/>
     </row>
-    <row r="211" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="211" s="1" customFormat="1" spans="6:12">
       <c r="F211" s="6"/>
       <c r="L211" s="6"/>
     </row>
-    <row r="212" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="212" s="1" customFormat="1" spans="6:12">
       <c r="F212" s="6"/>
       <c r="L212" s="6"/>
     </row>
-    <row r="213" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="213" s="1" customFormat="1" spans="6:12">
       <c r="F213" s="6"/>
       <c r="L213" s="6"/>
     </row>
-    <row r="214" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="214" s="1" customFormat="1" spans="6:12">
       <c r="F214" s="6"/>
       <c r="L214" s="6"/>
     </row>
-    <row r="215" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="215" s="1" customFormat="1" spans="6:12">
       <c r="F215" s="6"/>
       <c r="L215" s="6"/>
     </row>
-    <row r="216" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="216" s="1" customFormat="1" spans="6:12">
       <c r="F216" s="6"/>
       <c r="L216" s="6"/>
     </row>
-    <row r="217" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="217" s="1" customFormat="1" spans="6:12">
       <c r="F217" s="6"/>
       <c r="L217" s="6"/>
     </row>
-    <row r="218" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="218" s="1" customFormat="1" spans="6:12">
       <c r="F218" s="6"/>
       <c r="L218" s="6"/>
     </row>
-    <row r="219" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="219" s="1" customFormat="1" spans="6:12">
       <c r="F219" s="6"/>
       <c r="L219" s="6"/>
     </row>
-    <row r="220" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="220" s="1" customFormat="1" spans="6:12">
       <c r="F220" s="6"/>
       <c r="L220" s="6"/>
     </row>
-    <row r="221" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="221" s="1" customFormat="1" spans="6:12">
       <c r="F221" s="6"/>
       <c r="L221" s="6"/>
     </row>
-    <row r="222" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="222" s="1" customFormat="1" spans="6:12">
       <c r="F222" s="6"/>
       <c r="L222" s="6"/>
     </row>
-    <row r="223" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="223" s="1" customFormat="1" spans="6:12">
       <c r="F223" s="6"/>
       <c r="L223" s="6"/>
     </row>
-    <row r="224" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="224" s="1" customFormat="1" spans="6:12">
       <c r="F224" s="6"/>
       <c r="L224" s="6"/>
     </row>
-    <row r="225" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="225" s="1" customFormat="1" spans="6:12">
       <c r="F225" s="6"/>
       <c r="L225" s="6"/>
     </row>
-    <row r="226" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="226" s="1" customFormat="1" spans="6:12">
       <c r="F226" s="6"/>
       <c r="L226" s="6"/>
     </row>
-    <row r="227" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="227" s="1" customFormat="1" spans="6:12">
       <c r="F227" s="6"/>
       <c r="L227" s="6"/>
     </row>
-    <row r="228" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="228" s="1" customFormat="1" spans="6:12">
       <c r="F228" s="6"/>
       <c r="L228" s="6"/>
     </row>
-    <row r="229" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="229" s="1" customFormat="1" spans="6:12">
       <c r="F229" s="6"/>
       <c r="L229" s="6"/>
     </row>
-    <row r="230" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="230" s="1" customFormat="1" spans="6:12">
       <c r="F230" s="6"/>
       <c r="L230" s="6"/>
     </row>
-    <row r="231" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="231" s="1" customFormat="1" spans="6:12">
       <c r="F231" s="6"/>
       <c r="L231" s="6"/>
     </row>
-    <row r="232" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="232" s="1" customFormat="1" spans="6:12">
       <c r="F232" s="6"/>
       <c r="L232" s="6"/>
     </row>
-    <row r="233" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="233" s="1" customFormat="1" spans="6:12">
       <c r="F233" s="6"/>
       <c r="L233" s="6"/>
     </row>
-    <row r="234" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="234" s="1" customFormat="1" spans="6:12">
       <c r="F234" s="6"/>
       <c r="L234" s="6"/>
     </row>
-    <row r="235" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="235" s="1" customFormat="1" spans="6:12">
       <c r="F235" s="6"/>
       <c r="L235" s="6"/>
     </row>
-    <row r="236" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="236" s="1" customFormat="1" spans="6:12">
       <c r="F236" s="6"/>
       <c r="L236" s="6"/>
     </row>
-    <row r="237" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="237" s="1" customFormat="1" spans="6:12">
       <c r="F237" s="6"/>
       <c r="L237" s="6"/>
     </row>
-    <row r="238" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="238" s="1" customFormat="1" spans="6:12">
       <c r="F238" s="6"/>
       <c r="L238" s="6"/>
     </row>
-    <row r="239" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="239" s="1" customFormat="1" spans="6:12">
       <c r="F239" s="6"/>
       <c r="L239" s="6"/>
     </row>
-    <row r="240" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="240" s="1" customFormat="1" spans="6:12">
       <c r="F240" s="6"/>
       <c r="L240" s="6"/>
     </row>
-    <row r="241" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="241" s="1" customFormat="1" spans="6:12">
       <c r="F241" s="6"/>
       <c r="L241" s="6"/>
     </row>
-    <row r="242" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="242" s="1" customFormat="1" spans="6:12">
       <c r="F242" s="6"/>
       <c r="L242" s="6"/>
     </row>
-    <row r="243" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="243" s="1" customFormat="1" spans="6:12">
       <c r="F243" s="6"/>
       <c r="L243" s="6"/>
     </row>
-    <row r="244" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="244" s="1" customFormat="1" spans="6:12">
       <c r="F244" s="6"/>
       <c r="L244" s="6"/>
     </row>
-    <row r="245" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="245" s="1" customFormat="1" spans="6:12">
       <c r="F245" s="6"/>
       <c r="L245" s="6"/>
     </row>
-    <row r="246" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="246" s="1" customFormat="1" spans="6:12">
       <c r="F246" s="6"/>
       <c r="L246" s="6"/>
     </row>
-    <row r="247" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="247" s="1" customFormat="1" spans="6:12">
       <c r="F247" s="6"/>
       <c r="L247" s="6"/>
     </row>
-    <row r="248" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="248" s="1" customFormat="1" spans="6:12">
       <c r="F248" s="6"/>
       <c r="L248" s="6"/>
     </row>
-    <row r="249" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="249" s="1" customFormat="1" spans="6:12">
       <c r="F249" s="6"/>
       <c r="L249" s="6"/>
     </row>
-    <row r="250" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="250" s="1" customFormat="1" spans="6:12">
       <c r="F250" s="6"/>
       <c r="L250" s="6"/>
     </row>
-    <row r="251" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="251" s="1" customFormat="1" spans="6:12">
       <c r="F251" s="6"/>
       <c r="L251" s="6"/>
     </row>
-    <row r="252" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="252" s="1" customFormat="1" spans="6:12">
       <c r="F252" s="6"/>
       <c r="L252" s="6"/>
     </row>
-    <row r="253" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="253" s="1" customFormat="1" spans="6:12">
       <c r="F253" s="6"/>
       <c r="L253" s="6"/>
     </row>
-    <row r="254" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="254" s="1" customFormat="1" spans="6:12">
       <c r="F254" s="6"/>
       <c r="L254" s="6"/>
     </row>
-    <row r="255" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="255" s="1" customFormat="1" spans="6:12">
       <c r="F255" s="6"/>
       <c r="L255" s="6"/>
     </row>
-    <row r="256" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="256" s="1" customFormat="1" spans="6:12">
       <c r="F256" s="6"/>
       <c r="L256" s="6"/>
     </row>
-    <row r="257" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="257" s="1" customFormat="1" spans="6:12">
       <c r="F257" s="6"/>
       <c r="L257" s="6"/>
     </row>
-    <row r="258" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="258" s="1" customFormat="1" spans="6:12">
       <c r="F258" s="6"/>
       <c r="L258" s="6"/>
     </row>
-    <row r="259" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="259" s="1" customFormat="1" spans="6:12">
       <c r="F259" s="6"/>
       <c r="L259" s="6"/>
     </row>
-    <row r="260" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="260" s="1" customFormat="1" spans="6:12">
       <c r="F260" s="6"/>
       <c r="L260" s="6"/>
     </row>
-    <row r="261" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="261" s="1" customFormat="1" spans="6:12">
       <c r="F261" s="6"/>
       <c r="L261" s="6"/>
     </row>
-    <row r="262" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="262" s="1" customFormat="1" spans="6:12">
       <c r="F262" s="6"/>
       <c r="L262" s="6"/>
     </row>
-    <row r="263" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="263" s="1" customFormat="1" spans="6:12">
       <c r="F263" s="6"/>
       <c r="L263" s="6"/>
     </row>
-    <row r="264" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="264" s="1" customFormat="1" spans="6:12">
       <c r="F264" s="6"/>
       <c r="L264" s="6"/>
     </row>
-    <row r="265" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="265" s="1" customFormat="1" spans="6:12">
       <c r="F265" s="6"/>
       <c r="L265" s="6"/>
     </row>
-    <row r="266" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="266" s="1" customFormat="1" spans="6:12">
       <c r="F266" s="6"/>
       <c r="L266" s="6"/>
     </row>
-    <row r="267" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="267" s="1" customFormat="1" spans="6:12">
       <c r="F267" s="6"/>
       <c r="L267" s="6"/>
     </row>
-    <row r="268" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="268" s="1" customFormat="1" spans="6:12">
       <c r="F268" s="6"/>
       <c r="L268" s="6"/>
     </row>
-    <row r="269" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="269" s="1" customFormat="1" spans="6:12">
       <c r="F269" s="6"/>
       <c r="L269" s="6"/>
     </row>
-    <row r="270" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="270" s="1" customFormat="1" spans="6:12">
       <c r="F270" s="6"/>
       <c r="L270" s="6"/>
     </row>
-    <row r="271" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="271" s="1" customFormat="1" spans="6:12">
       <c r="F271" s="6"/>
       <c r="L271" s="6"/>
     </row>
-    <row r="272" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="272" s="1" customFormat="1" spans="6:12">
       <c r="F272" s="6"/>
       <c r="L272" s="6"/>
     </row>
-    <row r="273" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="273" s="1" customFormat="1" spans="6:12">
       <c r="F273" s="6"/>
       <c r="L273" s="6"/>
     </row>
-    <row r="274" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="274" s="1" customFormat="1" spans="6:12">
       <c r="F274" s="6"/>
       <c r="L274" s="6"/>
     </row>
-    <row r="275" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="275" s="1" customFormat="1" spans="6:12">
       <c r="F275" s="6"/>
       <c r="L275" s="6"/>
     </row>
-    <row r="276" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="276" s="1" customFormat="1" spans="6:12">
       <c r="F276" s="6"/>
       <c r="L276" s="6"/>
     </row>
-    <row r="277" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="277" s="1" customFormat="1" spans="6:12">
       <c r="F277" s="6"/>
       <c r="L277" s="6"/>
     </row>
-    <row r="278" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="278" s="1" customFormat="1" spans="6:12">
       <c r="F278" s="6"/>
       <c r="L278" s="6"/>
     </row>
-    <row r="279" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="279" s="1" customFormat="1" spans="6:12">
       <c r="F279" s="6"/>
       <c r="L279" s="6"/>
     </row>
-    <row r="280" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="280" s="1" customFormat="1" spans="6:12">
       <c r="F280" s="6"/>
       <c r="L280" s="6"/>
     </row>
-    <row r="281" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="281" s="1" customFormat="1" spans="6:12">
       <c r="F281" s="6"/>
       <c r="L281" s="6"/>
     </row>
-    <row r="282" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="282" s="1" customFormat="1" spans="6:12">
       <c r="F282" s="6"/>
       <c r="L282" s="6"/>
     </row>
-    <row r="283" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="283" s="1" customFormat="1" spans="6:12">
       <c r="F283" s="6"/>
       <c r="L283" s="6"/>
     </row>
-    <row r="284" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="284" s="1" customFormat="1" spans="6:12">
       <c r="F284" s="6"/>
       <c r="L284" s="6"/>
     </row>
-    <row r="285" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="285" s="1" customFormat="1" spans="6:12">
       <c r="F285" s="6"/>
       <c r="L285" s="6"/>
     </row>
-    <row r="286" s="1" customFormat="1" ht="14.25" spans="6:12">
+    <row r="286" s="1" customFormat="1" spans="6:12">
       <c r="F286" s="6"/>
       <c r="L286" s="6"/>
     </row>

</xml_diff>